<commit_message>
time 1 mass loss
</commit_message>
<xml_diff>
--- a/raw_data/pv_curves.xlsx
+++ b/raw_data/pv_curves.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="11">
   <si>
     <t>species</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>psi_bars</t>
+  </si>
+  <si>
+    <t>dry_mass_g</t>
   </si>
 </sst>
 </file>
@@ -96,10 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I58" sqref="I58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +431,7 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -449,8 +453,11 @@
       <c r="G1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -473,7 +480,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -496,7 +503,7 @@
         <v>3.1</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -519,7 +526,7 @@
         <v>3.3</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -542,7 +549,7 @@
         <v>4.0999999999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -565,7 +572,7 @@
         <v>4.4000000000000004</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -588,7 +595,7 @@
         <v>9.9</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
@@ -611,7 +618,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
@@ -634,7 +641,7 @@
         <v>9.1999999999999993</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
@@ -657,7 +664,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -680,7 +687,7 @@
         <v>9.1</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -703,7 +710,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -726,7 +733,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -749,7 +756,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
@@ -772,7 +779,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
more data entry for day 2
</commit_message>
<xml_diff>
--- a/raw_data/pv_curves.xlsx
+++ b/raw_data/pv_curves.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="17">
   <si>
     <t>species</t>
   </si>
@@ -44,9 +44,6 @@
     <t>laselva</t>
   </si>
   <si>
-    <t>phlebodium</t>
-  </si>
-  <si>
     <t>epiphyte</t>
   </si>
   <si>
@@ -57,6 +54,27 @@
   </si>
   <si>
     <t>dry_mass_g</t>
+  </si>
+  <si>
+    <t>phlebodium_aurem</t>
+  </si>
+  <si>
+    <t>thelypteris_curta</t>
+  </si>
+  <si>
+    <t>terrestrial</t>
+  </si>
+  <si>
+    <t>qc</t>
+  </si>
+  <si>
+    <t>bad</t>
+  </si>
+  <si>
+    <t>good</t>
+  </si>
+  <si>
+    <t>init</t>
   </si>
 </sst>
 </file>
@@ -418,20 +436,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:I126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="L124" sqref="L124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="5" width="9.140625" style="1"/>
+    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -448,27 +468,30 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2">
         <v>42832</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" s="1">
         <v>1</v>
@@ -479,19 +502,22 @@
       <c r="G2" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="2">
         <v>42832</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E3" s="1">
         <v>1</v>
@@ -502,19 +528,22 @@
       <c r="G3" s="1">
         <v>3.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I3" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="2">
         <v>42832</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>6</v>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -525,19 +554,22 @@
       <c r="G4" s="1">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="2">
         <v>42832</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="1">
         <v>1</v>
@@ -548,19 +580,22 @@
       <c r="G5" s="1">
         <v>4.0999999999999996</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="2">
         <v>42832</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>6</v>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -571,19 +606,22 @@
       <c r="G6" s="1">
         <v>4.4000000000000004</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I6" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>42832</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>6</v>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E7" s="1">
         <v>1</v>
@@ -594,19 +632,22 @@
       <c r="G7" s="1">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2">
         <v>42832</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>6</v>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" s="1">
         <v>2</v>
@@ -617,19 +658,22 @@
       <c r="G8" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2">
         <v>42832</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>6</v>
+      <c r="C9" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -640,19 +684,22 @@
       <c r="G9" s="1">
         <v>9.1999999999999993</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I9" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="2">
         <v>42832</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>6</v>
+      <c r="C10" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" s="1">
         <v>2</v>
@@ -663,19 +710,22 @@
       <c r="G10" s="1">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="2">
         <v>42832</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>6</v>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E11" s="1">
         <v>2</v>
@@ -686,19 +736,22 @@
       <c r="G11" s="1">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I11" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="2">
         <v>42832</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>6</v>
+      <c r="C12" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" s="1">
         <v>2</v>
@@ -709,19 +762,22 @@
       <c r="G12" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="2">
         <v>42832</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>6</v>
+      <c r="C13" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E13" s="1">
         <v>2</v>
@@ -732,19 +788,22 @@
       <c r="G13" s="1">
         <v>9.5</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="2">
         <v>42832</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>6</v>
+      <c r="C14" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -755,19 +814,22 @@
       <c r="G14" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="2">
         <v>42832</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>6</v>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -778,19 +840,22 @@
       <c r="G15" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I15" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="2">
         <v>42832</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>6</v>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
@@ -801,19 +866,22 @@
       <c r="G16" s="1">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I16" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="2">
         <v>42832</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>6</v>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -824,19 +892,22 @@
       <c r="G17" s="1">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="2">
         <v>42832</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>6</v>
+      <c r="C18" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
@@ -847,19 +918,22 @@
       <c r="G18" s="1">
         <v>12.9</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="2">
         <v>42832</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>6</v>
+      <c r="C19" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E19" s="1">
         <v>3</v>
@@ -870,19 +944,22 @@
       <c r="G19" s="1">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="2">
         <v>42832</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>6</v>
+      <c r="C20" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E20" s="1">
         <v>3</v>
@@ -893,19 +970,22 @@
       <c r="G20" s="1">
         <v>6.8</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="2">
         <v>42832</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>6</v>
+      <c r="C21" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E21" s="1">
         <v>3</v>
@@ -916,19 +996,22 @@
       <c r="G21" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I21" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="2">
         <v>42832</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>6</v>
+      <c r="C22" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E22" s="1">
         <v>3</v>
@@ -939,19 +1022,22 @@
       <c r="G22" s="1">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I22" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="2">
         <v>42832</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>6</v>
+      <c r="C23" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E23" s="1">
         <v>3</v>
@@ -962,19 +1048,22 @@
       <c r="G23" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I23" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="2">
         <v>42832</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>6</v>
+      <c r="C24" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E24" s="1">
         <v>3</v>
@@ -985,19 +1074,22 @@
       <c r="G24" s="1">
         <v>7.7</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I24" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="2">
         <v>42832</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
+      <c r="C25" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25" s="1">
         <v>3</v>
@@ -1008,19 +1100,22 @@
       <c r="G25" s="1">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I25" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B26" s="2">
         <v>42832</v>
       </c>
-      <c r="C26" s="1" t="s">
-        <v>6</v>
+      <c r="C26" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E26" s="1">
         <v>3</v>
@@ -1031,19 +1126,22 @@
       <c r="G26" s="1">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I26" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B27" s="2">
         <v>42832</v>
       </c>
-      <c r="C27" s="1" t="s">
-        <v>6</v>
+      <c r="C27" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" s="1">
         <v>3</v>
@@ -1054,19 +1152,22 @@
       <c r="G27" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I27" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B28" s="2">
         <v>42832</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>6</v>
+      <c r="C28" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28" s="1">
         <v>4</v>
@@ -1077,19 +1178,22 @@
       <c r="G28" s="1">
         <v>6.2</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I28" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B29" s="2">
         <v>42832</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>6</v>
+      <c r="C29" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E29" s="1">
         <v>4</v>
@@ -1100,19 +1204,22 @@
       <c r="G29" s="1">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I29" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B30" s="2">
         <v>42832</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>6</v>
+      <c r="C30" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30" s="1">
         <v>4</v>
@@ -1123,19 +1230,22 @@
       <c r="G30" s="1">
         <v>7.1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I30" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B31" s="2">
         <v>42832</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>6</v>
+      <c r="C31" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31" s="1">
         <v>4</v>
@@ -1146,19 +1256,22 @@
       <c r="G31" s="1">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I31" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B32" s="2">
         <v>42832</v>
       </c>
-      <c r="C32" s="1" t="s">
-        <v>6</v>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E32" s="1">
         <v>4</v>
@@ -1169,19 +1282,22 @@
       <c r="G32" s="1">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I32" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B33" s="2">
         <v>42832</v>
       </c>
-      <c r="C33" s="1" t="s">
-        <v>6</v>
+      <c r="C33" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E33" s="1">
         <v>4</v>
@@ -1192,19 +1308,22 @@
       <c r="G33" s="1">
         <v>7.9</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I33" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B34" s="2">
         <v>42832</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>6</v>
+      <c r="C34" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E34" s="1">
         <v>4</v>
@@ -1215,19 +1334,22 @@
       <c r="G34" s="1">
         <v>8.1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I34" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B35" s="2">
         <v>42832</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>6</v>
+      <c r="C35" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E35" s="1">
         <v>4</v>
@@ -1238,19 +1360,22 @@
       <c r="G35" s="1">
         <v>9</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I35" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B36" s="2">
         <v>42832</v>
       </c>
-      <c r="C36" s="1" t="s">
-        <v>6</v>
+      <c r="C36" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E36" s="1">
         <v>5</v>
@@ -1261,19 +1386,22 @@
       <c r="G36" s="1">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I36" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B37" s="2">
         <v>42832</v>
       </c>
-      <c r="C37" s="1" t="s">
-        <v>6</v>
+      <c r="C37" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E37" s="1">
         <v>5</v>
@@ -1284,19 +1412,22 @@
       <c r="G37" s="1">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I37" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B38" s="2">
         <v>42832</v>
       </c>
-      <c r="C38" s="1" t="s">
-        <v>6</v>
+      <c r="C38" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E38" s="1">
         <v>5</v>
@@ -1307,19 +1438,22 @@
       <c r="G38" s="1">
         <v>8.3000000000000007</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I38" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B39" s="2">
         <v>42832</v>
       </c>
-      <c r="C39" s="1" t="s">
-        <v>6</v>
+      <c r="C39" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E39" s="1">
         <v>5</v>
@@ -1330,19 +1464,22 @@
       <c r="G39" s="1">
         <v>9.9</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I39" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B40" s="2">
         <v>42832</v>
       </c>
-      <c r="C40" s="1" t="s">
-        <v>6</v>
+      <c r="C40" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E40" s="1">
         <v>5</v>
@@ -1353,19 +1490,22 @@
       <c r="G40" s="1">
         <v>10.199999999999999</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I40" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B41" s="2">
         <v>42832</v>
       </c>
-      <c r="C41" s="1" t="s">
-        <v>6</v>
+      <c r="C41" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E41" s="1">
         <v>5</v>
@@ -1376,19 +1516,22 @@
       <c r="G41" s="1">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I41" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B42" s="2">
         <v>42832</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>6</v>
+      <c r="C42" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E42" s="1">
         <v>5</v>
@@ -1399,19 +1542,22 @@
       <c r="G42" s="1">
         <v>13.1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B43" s="2">
         <v>42832</v>
       </c>
-      <c r="C43" s="1" t="s">
-        <v>6</v>
+      <c r="C43" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E43" s="1">
         <v>5</v>
@@ -1422,19 +1568,22 @@
       <c r="G43" s="1">
         <v>13.9</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I43" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B44" s="2">
         <v>42832</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>6</v>
+      <c r="C44" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E44" s="1">
         <v>6</v>
@@ -1445,19 +1594,22 @@
       <c r="G44" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B45" s="2">
         <v>42832</v>
       </c>
-      <c r="C45" s="1" t="s">
-        <v>6</v>
+      <c r="C45" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E45" s="1">
         <v>6</v>
@@ -1468,19 +1620,22 @@
       <c r="G45" s="1">
         <v>5.5</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I45" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B46" s="2">
         <v>42832</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>6</v>
+      <c r="C46" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E46" s="1">
         <v>6</v>
@@ -1491,19 +1646,22 @@
       <c r="G46" s="1">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I46" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B47" s="2">
         <v>42832</v>
       </c>
-      <c r="C47" s="1" t="s">
-        <v>6</v>
+      <c r="C47" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E47" s="1">
         <v>6</v>
@@ -1514,19 +1672,22 @@
       <c r="G47" s="1">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I47" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B48" s="2">
         <v>42832</v>
       </c>
-      <c r="C48" s="1" t="s">
-        <v>6</v>
+      <c r="C48" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E48" s="1">
         <v>6</v>
@@ -1537,19 +1698,22 @@
       <c r="G48" s="1">
         <v>6.5</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I48" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B49" s="2">
         <v>42832</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>6</v>
+      <c r="C49" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E49" s="1">
         <v>6</v>
@@ -1560,19 +1724,22 @@
       <c r="G49" s="1">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I49" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B50" s="2">
         <v>42832</v>
       </c>
-      <c r="C50" s="1" t="s">
-        <v>6</v>
+      <c r="C50" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E50" s="1">
         <v>6</v>
@@ -1583,19 +1750,22 @@
       <c r="G50" s="1">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I50" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B51" s="2">
         <v>42832</v>
       </c>
-      <c r="C51" s="1" t="s">
-        <v>6</v>
+      <c r="C51" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E51" s="1">
         <v>6</v>
@@ -1606,19 +1776,22 @@
       <c r="G51" s="1">
         <v>8.9</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I51" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B52" s="2">
         <v>42832</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>6</v>
+      <c r="C52" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E52" s="1">
         <v>6</v>
@@ -1629,19 +1802,22 @@
       <c r="G52" s="1">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I52" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B53" s="2">
         <v>42832</v>
       </c>
-      <c r="C53" s="1" t="s">
-        <v>6</v>
+      <c r="C53" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E53" s="1">
         <v>6</v>
@@ -1652,19 +1828,22 @@
       <c r="G53" s="1">
         <v>9.4</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I53" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B54" s="2">
         <v>42832</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>6</v>
+      <c r="C54" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E54" s="1">
         <v>6</v>
@@ -1675,19 +1854,22 @@
       <c r="G54" s="1">
         <v>11.9</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I54" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B55" s="2">
         <v>42832</v>
       </c>
-      <c r="C55" s="1" t="s">
-        <v>6</v>
+      <c r="C55" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E55" s="1">
         <v>7</v>
@@ -1698,19 +1880,22 @@
       <c r="G55" s="1">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I55" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B56" s="2">
         <v>42832</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>6</v>
+      <c r="C56" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E56" s="1">
         <v>7</v>
@@ -1721,19 +1906,22 @@
       <c r="G56" s="1">
         <v>4.8</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I56" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B57" s="2">
         <v>42832</v>
       </c>
-      <c r="C57" s="1" t="s">
-        <v>6</v>
+      <c r="C57" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E57" s="1">
         <v>7</v>
@@ -1744,19 +1932,22 @@
       <c r="G57" s="1">
         <v>5.0999999999999996</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I57" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B58" s="2">
         <v>42832</v>
       </c>
-      <c r="C58" s="1" t="s">
-        <v>6</v>
+      <c r="C58" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E58" s="1">
         <v>7</v>
@@ -1767,19 +1958,22 @@
       <c r="G58" s="1">
         <v>5.3</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I58" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B59" s="2">
         <v>42832</v>
       </c>
-      <c r="C59" s="1" t="s">
-        <v>6</v>
+      <c r="C59" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E59" s="1">
         <v>7</v>
@@ -1790,19 +1984,22 @@
       <c r="G59" s="1">
         <v>6.9</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I59" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B60" s="2">
         <v>42832</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>6</v>
+      <c r="C60" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E60" s="1">
         <v>7</v>
@@ -1813,19 +2010,22 @@
       <c r="G60" s="1">
         <v>7.2</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I60" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B61" s="2">
         <v>42832</v>
       </c>
-      <c r="C61" s="1" t="s">
-        <v>6</v>
+      <c r="C61" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E61" s="1">
         <v>7</v>
@@ -1836,19 +2036,22 @@
       <c r="G61" s="1">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I61" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B62" s="2">
         <v>42832</v>
       </c>
-      <c r="C62" s="1" t="s">
-        <v>6</v>
+      <c r="C62" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E62" s="1">
         <v>7</v>
@@ -1859,19 +2062,22 @@
       <c r="G62" s="1">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I62" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B63" s="2">
         <v>42832</v>
       </c>
-      <c r="C63" s="1" t="s">
-        <v>6</v>
+      <c r="C63" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E63" s="1">
         <v>7</v>
@@ -1882,19 +2088,22 @@
       <c r="G63" s="1">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I63" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B64" s="2">
         <v>42832</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>6</v>
+      <c r="C64" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E64" s="1">
         <v>8</v>
@@ -1905,19 +2114,22 @@
       <c r="G64" s="1">
         <v>2.9</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I64" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B65" s="2">
         <v>42832</v>
       </c>
-      <c r="C65" s="1" t="s">
-        <v>6</v>
+      <c r="C65" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E65" s="1">
         <v>8</v>
@@ -1928,19 +2140,22 @@
       <c r="G65" s="1">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I65" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B66" s="2">
         <v>42832</v>
       </c>
-      <c r="C66" s="1" t="s">
-        <v>6</v>
+      <c r="C66" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E66" s="1">
         <v>8</v>
@@ -1951,19 +2166,22 @@
       <c r="G66" s="1">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I66" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B67" s="2">
         <v>42832</v>
       </c>
-      <c r="C67" s="1" t="s">
-        <v>6</v>
+      <c r="C67" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E67" s="1">
         <v>8</v>
@@ -1974,19 +2192,22 @@
       <c r="G67" s="1">
         <v>5.4</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I67" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B68" s="2">
         <v>42832</v>
       </c>
-      <c r="C68" s="1" t="s">
-        <v>6</v>
+      <c r="C68" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E68" s="1">
         <v>8</v>
@@ -1997,19 +2218,22 @@
       <c r="G68" s="1">
         <v>6.1</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I68" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B69" s="2">
         <v>42832</v>
       </c>
-      <c r="C69" s="1" t="s">
-        <v>6</v>
+      <c r="C69" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E69" s="1">
         <v>8</v>
@@ -2020,19 +2244,22 @@
       <c r="G69" s="1">
         <v>6.6</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I69" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B70" s="2">
         <v>42832</v>
       </c>
-      <c r="C70" s="1" t="s">
-        <v>6</v>
+      <c r="C70" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E70" s="1">
         <v>8</v>
@@ -2043,19 +2270,22 @@
       <c r="G70" s="1">
         <v>7</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I70" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B71" s="2">
         <v>42832</v>
       </c>
-      <c r="C71" s="1" t="s">
-        <v>6</v>
+      <c r="C71" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E71" s="1">
         <v>8</v>
@@ -2066,19 +2296,22 @@
       <c r="G71" s="1">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I71" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B72" s="2">
         <v>42832</v>
       </c>
-      <c r="C72" s="1" t="s">
-        <v>6</v>
+      <c r="C72" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E72" s="1">
         <v>8</v>
@@ -2088,6 +2321,1413 @@
       </c>
       <c r="G72" s="1">
         <v>10.8</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B73" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D73" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E73" s="3">
+        <v>1</v>
+      </c>
+      <c r="F73" s="3">
+        <v>1.4</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B74" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D74" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E74" s="3">
+        <v>1</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1.3617999999999999</v>
+      </c>
+      <c r="G74" s="3">
+        <v>2</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B75" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E75" s="3">
+        <v>1</v>
+      </c>
+      <c r="F75" s="3">
+        <v>1.3169999999999999</v>
+      </c>
+      <c r="G75" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E76" s="3">
+        <v>1</v>
+      </c>
+      <c r="F76" s="3">
+        <v>1.3081</v>
+      </c>
+      <c r="G76" s="3">
+        <v>6.1</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E77" s="3">
+        <v>1</v>
+      </c>
+      <c r="F77" s="3">
+        <v>1.2939000000000001</v>
+      </c>
+      <c r="G77" s="3">
+        <v>9</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B78" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E78" s="3">
+        <v>1</v>
+      </c>
+      <c r="F78" s="3">
+        <v>1.2675000000000001</v>
+      </c>
+      <c r="G78" s="3">
+        <v>11.2</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" s="3">
+        <v>1</v>
+      </c>
+      <c r="F79" s="3">
+        <v>1.2148000000000001</v>
+      </c>
+      <c r="G79" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="I79" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B80" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" s="3">
+        <v>1</v>
+      </c>
+      <c r="F80" s="3">
+        <v>1.1744000000000001</v>
+      </c>
+      <c r="G80" s="3">
+        <v>14</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B81" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E81" s="3">
+        <v>1</v>
+      </c>
+      <c r="F81" s="3">
+        <v>1.1021000000000001</v>
+      </c>
+      <c r="G81" s="3">
+        <v>15.8</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B82" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E82" s="3">
+        <v>2</v>
+      </c>
+      <c r="F82" s="3">
+        <v>1.4400999999999999</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B83" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E83" s="3">
+        <v>2</v>
+      </c>
+      <c r="F83" s="3">
+        <v>1.4008</v>
+      </c>
+      <c r="G83" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B84" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C84" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E84" s="3">
+        <v>2</v>
+      </c>
+      <c r="F84" s="3">
+        <v>1.3717999999999999</v>
+      </c>
+      <c r="G84" s="3">
+        <v>6</v>
+      </c>
+      <c r="I84" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B85" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D85" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E85" s="3">
+        <v>2</v>
+      </c>
+      <c r="F85" s="3">
+        <v>1.3625</v>
+      </c>
+      <c r="G85" s="3">
+        <v>9</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B86" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C86" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E86" s="3">
+        <v>2</v>
+      </c>
+      <c r="F86" s="3">
+        <v>1.35</v>
+      </c>
+      <c r="G86" s="3">
+        <v>10.5</v>
+      </c>
+      <c r="I86" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E87" s="3">
+        <v>2</v>
+      </c>
+      <c r="F87" s="3">
+        <v>1.3230999999999999</v>
+      </c>
+      <c r="G87" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="I87" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C88" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E88" s="3">
+        <v>2</v>
+      </c>
+      <c r="F88" s="3">
+        <v>1.274</v>
+      </c>
+      <c r="G88" s="3">
+        <v>13</v>
+      </c>
+      <c r="I88" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B89" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C89" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E89" s="3">
+        <v>2</v>
+      </c>
+      <c r="F89" s="3">
+        <v>1.2194</v>
+      </c>
+      <c r="G89" s="3">
+        <v>14</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B90" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C90" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E90" s="3">
+        <v>2</v>
+      </c>
+      <c r="F90" s="3">
+        <v>1.1798999999999999</v>
+      </c>
+      <c r="G90" s="3">
+        <v>14.8</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A91" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B91" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" s="3">
+        <v>3</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0.98370000000000002</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I91" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A92" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C92" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D92" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" s="3">
+        <v>3</v>
+      </c>
+      <c r="F92" s="3">
+        <v>0.9617</v>
+      </c>
+      <c r="G92" s="3">
+        <v>3</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E93" s="3">
+        <v>3</v>
+      </c>
+      <c r="F93" s="3">
+        <v>0.94399999999999995</v>
+      </c>
+      <c r="G93" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B94" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="3">
+        <v>3</v>
+      </c>
+      <c r="F94" s="3">
+        <v>0.93340000000000001</v>
+      </c>
+      <c r="G94" s="3">
+        <v>11.1</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B95" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C95" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E95" s="3">
+        <v>3</v>
+      </c>
+      <c r="F95" s="3">
+        <v>0.92589999999999995</v>
+      </c>
+      <c r="G95" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B96" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C96" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E96" s="3">
+        <v>3</v>
+      </c>
+      <c r="F96" s="3">
+        <v>0.90710000000000002</v>
+      </c>
+      <c r="G96" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A97" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B97" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E97" s="3">
+        <v>3</v>
+      </c>
+      <c r="F97" s="3">
+        <v>0.87460000000000004</v>
+      </c>
+      <c r="G97" s="3">
+        <v>14.2</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B98" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E98" s="3">
+        <v>3</v>
+      </c>
+      <c r="F98" s="3">
+        <v>0.8488</v>
+      </c>
+      <c r="G98" s="3">
+        <v>14.9</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E99" s="3">
+        <v>4</v>
+      </c>
+      <c r="F99" s="3">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B100" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="3">
+        <v>4</v>
+      </c>
+      <c r="F100" s="3">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="G100" s="3">
+        <v>3</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A101" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B101" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C101" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E101" s="3">
+        <v>4</v>
+      </c>
+      <c r="F101" s="3">
+        <v>0.92090000000000005</v>
+      </c>
+      <c r="G101" s="3">
+        <v>6</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B102" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C102" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" s="3">
+        <v>4</v>
+      </c>
+      <c r="F102" s="3">
+        <v>0.88539999999999996</v>
+      </c>
+      <c r="G102" s="3">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A103" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B103" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C103" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" s="3">
+        <v>4</v>
+      </c>
+      <c r="F103" s="3">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="G103" s="3">
+        <v>12.5</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A104" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C104" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E104" s="3">
+        <v>4</v>
+      </c>
+      <c r="F104" s="3">
+        <v>0.75319999999999998</v>
+      </c>
+      <c r="G104" s="3">
+        <v>14.1</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A105" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B105" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C105" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" s="3">
+        <v>4</v>
+      </c>
+      <c r="F105" s="3">
+        <v>0.71179999999999999</v>
+      </c>
+      <c r="G105" s="3">
+        <v>15.9</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B106" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C106" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E106" s="3">
+        <v>4</v>
+      </c>
+      <c r="F106" s="3">
+        <v>0.68689999999999996</v>
+      </c>
+      <c r="G106" s="3">
+        <v>17</v>
+      </c>
+      <c r="I106" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B107" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C107" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E107" s="3">
+        <v>5</v>
+      </c>
+      <c r="F107" s="3">
+        <v>1.0720000000000001</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I107" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A108" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B108" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C108" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108" s="3">
+        <v>5</v>
+      </c>
+      <c r="F108" s="3">
+        <v>1.0527</v>
+      </c>
+      <c r="G108" s="3">
+        <v>3.8</v>
+      </c>
+      <c r="I108" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B109" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C109" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109" s="3">
+        <v>5</v>
+      </c>
+      <c r="F109" s="3">
+        <v>1.0401</v>
+      </c>
+      <c r="G109" s="3">
+        <v>7.5</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A110" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C110" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" s="3">
+        <v>5</v>
+      </c>
+      <c r="F110" s="3">
+        <v>1.0263</v>
+      </c>
+      <c r="G110" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B111" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C111" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E111" s="3">
+        <v>5</v>
+      </c>
+      <c r="F111" s="3">
+        <v>1.0129999999999999</v>
+      </c>
+      <c r="G111" s="3">
+        <v>9.6</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A112" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E112" s="3">
+        <v>5</v>
+      </c>
+      <c r="F112" s="3">
+        <v>1.0016</v>
+      </c>
+      <c r="G112" s="3">
+        <v>10.4</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A113" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B113" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C113" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D113" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E113" s="3">
+        <v>5</v>
+      </c>
+      <c r="F113" s="3">
+        <v>0.97799999999999998</v>
+      </c>
+      <c r="G113" s="3">
+        <v>11</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B114" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C114" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E114" s="3">
+        <v>5</v>
+      </c>
+      <c r="F114" s="3">
+        <v>0.94530000000000003</v>
+      </c>
+      <c r="G114" s="3">
+        <v>11.8</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B115" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C115" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D115" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E115" s="3">
+        <v>5</v>
+      </c>
+      <c r="F115" s="3">
+        <v>0.92830000000000001</v>
+      </c>
+      <c r="G115" s="3">
+        <v>12.7</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A116" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B116" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C116" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E116" s="3">
+        <v>5</v>
+      </c>
+      <c r="F116" s="3">
+        <v>0.67859999999999998</v>
+      </c>
+      <c r="G116" s="3">
+        <v>18</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A117" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B117" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C117" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E117" s="3">
+        <v>6</v>
+      </c>
+      <c r="F117" s="3">
+        <v>1.3303</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I117" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A118" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B118" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C118" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E118" s="3">
+        <v>6</v>
+      </c>
+      <c r="F118" s="3">
+        <v>1.3078000000000001</v>
+      </c>
+      <c r="G118" s="3">
+        <v>3.2</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B119" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C119" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E119" s="3">
+        <v>6</v>
+      </c>
+      <c r="F119" s="3">
+        <v>1.2905</v>
+      </c>
+      <c r="G119" s="3">
+        <v>11</v>
+      </c>
+      <c r="I119" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A120" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C120" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D120" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120" s="3">
+        <v>6</v>
+      </c>
+      <c r="F120" s="3">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="G120" s="3">
+        <v>9.9</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A121" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C121" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" s="3">
+        <v>6</v>
+      </c>
+      <c r="F121" s="3">
+        <v>1.2632000000000001</v>
+      </c>
+      <c r="G121" s="3">
+        <v>12.1</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A122" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B122" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C122" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E122" s="3">
+        <v>6</v>
+      </c>
+      <c r="F122" s="3">
+        <v>1.2184999999999999</v>
+      </c>
+      <c r="G122" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B123" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E123" s="3">
+        <v>6</v>
+      </c>
+      <c r="F123" s="3">
+        <v>1.1572</v>
+      </c>
+      <c r="G123" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A124" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B124" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C124" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E124" s="3">
+        <v>6</v>
+      </c>
+      <c r="F124" s="3">
+        <v>1.0678000000000001</v>
+      </c>
+      <c r="G124" s="3">
+        <v>14.2</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A125" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B125" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E125" s="3">
+        <v>6</v>
+      </c>
+      <c r="F125" s="3">
+        <v>1.0306</v>
+      </c>
+      <c r="G125" s="3">
+        <v>16.100000000000001</v>
+      </c>
+      <c r="I125" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A126" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B126" s="2">
+        <v>42893</v>
+      </c>
+      <c r="C126" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E126" s="3">
+        <v>6</v>
+      </c>
+      <c r="F126" s="3">
+        <v>0.77110000000000001</v>
+      </c>
+      <c r="G126" s="3">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more data entry 7/13/17
</commit_message>
<xml_diff>
--- a/raw_data/pv_curves.xlsx
+++ b/raw_data/pv_curves.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2385" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="34">
   <si>
     <t>species</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>dry_mass_g</t>
+  </si>
+  <si>
+    <t>cyclopeltis_semicordata</t>
+  </si>
+  <si>
+    <t>mickelia_nicotianifolia</t>
   </si>
 </sst>
 </file>
@@ -482,11 +488,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P684"/>
+  <dimension ref="A1:P810"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A664" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C467" sqref="C467:D470"/>
+      <pane ySplit="1" topLeftCell="A781" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H800" sqref="H800"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17917,7 +17923,7 @@
         <v>43015</v>
       </c>
       <c r="C673" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D673" s="3" t="s">
         <v>11</v>
@@ -17934,81 +17940,2873 @@
       <c r="H673" s="3"/>
     </row>
     <row r="674" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A674" s="3"/>
-      <c r="B674" s="2"/>
-      <c r="C674" s="3"/>
-      <c r="D674" s="3"/>
-      <c r="E674" s="3"/>
+      <c r="A674" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B674" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C674" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D674" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E674" s="3">
+        <v>1</v>
+      </c>
+      <c r="F674" s="3">
+        <v>1.8165</v>
+      </c>
+      <c r="G674" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="675" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A675" s="3"/>
-      <c r="B675" s="2"/>
-      <c r="C675" s="3"/>
-      <c r="D675" s="3"/>
-      <c r="E675" s="3"/>
+      <c r="A675" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B675" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C675" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D675" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E675" s="3">
+        <v>1</v>
+      </c>
+      <c r="F675" s="3">
+        <v>1.786</v>
+      </c>
+      <c r="G675" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="676" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A676" s="3"/>
-      <c r="B676" s="2"/>
-      <c r="C676" s="3"/>
-      <c r="D676" s="3"/>
-      <c r="E676" s="3"/>
+      <c r="A676" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B676" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C676" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D676" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E676" s="3">
+        <v>1</v>
+      </c>
+      <c r="F676" s="3">
+        <v>1.7697000000000001</v>
+      </c>
+      <c r="G676" s="3">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="677" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A677" s="3"/>
-      <c r="B677" s="2"/>
-      <c r="C677" s="3"/>
-      <c r="D677" s="3"/>
-      <c r="E677" s="3"/>
+      <c r="A677" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B677" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C677" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D677" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E677" s="3">
+        <v>1</v>
+      </c>
+      <c r="F677" s="3">
+        <v>1.7468999999999999</v>
+      </c>
+      <c r="G677" s="3">
+        <v>2.9</v>
+      </c>
     </row>
     <row r="678" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A678" s="3"/>
-      <c r="B678" s="2"/>
-      <c r="C678" s="3"/>
-      <c r="D678" s="3"/>
-      <c r="E678" s="3"/>
+      <c r="A678" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B678" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C678" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D678" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E678" s="3">
+        <v>1</v>
+      </c>
+      <c r="F678" s="3">
+        <v>1.7351000000000001</v>
+      </c>
+      <c r="G678" s="3">
+        <v>4.9000000000000004</v>
+      </c>
     </row>
     <row r="679" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A679" s="3"/>
-      <c r="B679" s="2"/>
-      <c r="C679" s="3"/>
-      <c r="D679" s="3"/>
-      <c r="E679" s="3"/>
+      <c r="A679" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B679" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C679" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D679" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E679" s="3">
+        <v>1</v>
+      </c>
+      <c r="F679" s="3">
+        <v>1.7222</v>
+      </c>
+      <c r="G679" s="3">
+        <v>6.2</v>
+      </c>
     </row>
     <row r="680" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A680" s="3"/>
-      <c r="B680" s="2"/>
-      <c r="C680" s="3"/>
-      <c r="D680" s="3"/>
-      <c r="E680" s="3"/>
+      <c r="A680" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B680" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C680" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D680" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E680" s="3">
+        <v>1</v>
+      </c>
+      <c r="F680" s="3">
+        <v>1.7124999999999999</v>
+      </c>
+      <c r="G680" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="681" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A681" s="3"/>
-      <c r="B681" s="2"/>
-      <c r="C681" s="3"/>
-      <c r="D681" s="3"/>
-      <c r="E681" s="3"/>
+      <c r="A681" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B681" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C681" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D681" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E681" s="3">
+        <v>1</v>
+      </c>
+      <c r="F681" s="3">
+        <v>1.6994</v>
+      </c>
+      <c r="G681" s="3">
+        <v>10</v>
+      </c>
     </row>
     <row r="682" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A682" s="3"/>
-      <c r="B682" s="2"/>
-      <c r="C682" s="3"/>
-      <c r="D682" s="3"/>
-      <c r="E682" s="3"/>
+      <c r="A682" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B682" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C682" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D682" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E682" s="3">
+        <v>1</v>
+      </c>
+      <c r="F682" s="3">
+        <v>0.69230000000000003</v>
+      </c>
+      <c r="G682" s="3">
+        <v>13.4</v>
+      </c>
     </row>
     <row r="683" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A683" s="3"/>
-      <c r="B683" s="2"/>
-      <c r="C683" s="3"/>
-      <c r="D683" s="3"/>
-      <c r="E683" s="3"/>
+      <c r="A683" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B683" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C683" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D683" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E683" s="3">
+        <v>1</v>
+      </c>
+      <c r="F683" s="3">
+        <v>1.6323000000000001</v>
+      </c>
+      <c r="G683" s="3">
+        <v>14.8</v>
+      </c>
     </row>
     <row r="684" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A684" s="3"/>
-      <c r="B684" s="2"/>
-      <c r="C684" s="3"/>
-      <c r="D684" s="3"/>
-      <c r="E684" s="3"/>
+      <c r="A684" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B684" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C684" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D684" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E684" s="3">
+        <v>1</v>
+      </c>
+      <c r="F684" s="3">
+        <v>1.6074999999999999</v>
+      </c>
+      <c r="G684" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="685" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A685" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B685" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C685" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D685" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E685" s="3">
+        <v>2</v>
+      </c>
+      <c r="F685" s="3">
+        <v>1.8046</v>
+      </c>
+      <c r="G685" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="686" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A686" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B686" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C686" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D686" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E686" s="3">
+        <v>2</v>
+      </c>
+      <c r="F686" s="3">
+        <v>1.7798</v>
+      </c>
+      <c r="G686" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="687" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A687" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B687" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C687" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D687" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E687" s="3">
+        <v>2</v>
+      </c>
+      <c r="F687" s="3">
+        <v>1.7661</v>
+      </c>
+      <c r="G687" s="3">
+        <v>2.9</v>
+      </c>
+    </row>
+    <row r="688" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A688" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B688" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C688" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D688" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E688" s="3">
+        <v>2</v>
+      </c>
+      <c r="F688" s="3">
+        <v>1.7155</v>
+      </c>
+      <c r="G688" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="689" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A689" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B689" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C689" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D689" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E689" s="3">
+        <v>2</v>
+      </c>
+      <c r="F689" s="3">
+        <v>1.7094</v>
+      </c>
+      <c r="G689" s="3">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="690" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A690" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B690" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C690" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D690" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E690" s="3">
+        <v>2</v>
+      </c>
+      <c r="F690" s="3">
+        <v>1.6989000000000001</v>
+      </c>
+      <c r="G690" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="691" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A691" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B691" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C691" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D691" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E691" s="3">
+        <v>2</v>
+      </c>
+      <c r="F691" s="3">
+        <v>1.6912</v>
+      </c>
+      <c r="G691" s="3">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="692" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A692" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B692" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C692" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D692" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E692" s="3">
+        <v>2</v>
+      </c>
+      <c r="F692" s="3">
+        <v>1.6855</v>
+      </c>
+      <c r="G692" s="3">
+        <v>7.9</v>
+      </c>
+    </row>
+    <row r="693" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A693" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B693" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C693" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D693" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E693" s="3">
+        <v>2</v>
+      </c>
+      <c r="F693" s="3">
+        <v>1.6762999999999999</v>
+      </c>
+      <c r="G693" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="694" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A694" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B694" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C694" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D694" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E694" s="3">
+        <v>2</v>
+      </c>
+      <c r="F694" s="3">
+        <v>1.6577</v>
+      </c>
+      <c r="G694" s="3">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="695" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A695" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B695" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C695" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D695" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E695" s="3">
+        <v>2</v>
+      </c>
+      <c r="F695" s="3">
+        <v>1.6398999999999999</v>
+      </c>
+      <c r="G695" s="3">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="696" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A696" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B696" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C696" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D696" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E696" s="3">
+        <v>2</v>
+      </c>
+      <c r="F696" s="3">
+        <v>1.6304000000000001</v>
+      </c>
+      <c r="G696" s="3">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="697" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A697" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B697" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C697" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D697" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E697" s="3">
+        <v>2</v>
+      </c>
+      <c r="F697" s="3">
+        <v>1.5028999999999999</v>
+      </c>
+      <c r="G697" s="3">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="698" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A698" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B698" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C698" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D698" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E698" s="3">
+        <v>3</v>
+      </c>
+      <c r="F698" s="3">
+        <v>4.0877999999999997</v>
+      </c>
+      <c r="G698" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="699" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A699" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B699" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C699" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D699" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E699" s="3">
+        <v>3</v>
+      </c>
+      <c r="F699" s="3">
+        <v>4.0572999999999997</v>
+      </c>
+      <c r="G699" s="3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="700" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A700" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B700" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C700" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D700" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E700" s="3">
+        <v>3</v>
+      </c>
+      <c r="F700" s="3">
+        <v>4.0373000000000001</v>
+      </c>
+      <c r="G700" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="701" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A701" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B701" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C701" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D701" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E701" s="3">
+        <v>3</v>
+      </c>
+      <c r="F701" s="3">
+        <v>4.0237999999999996</v>
+      </c>
+      <c r="G701" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="702" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A702" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B702" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C702" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D702" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E702" s="3">
+        <v>3</v>
+      </c>
+      <c r="F702" s="3">
+        <v>4.0101000000000004</v>
+      </c>
+      <c r="G702" s="3">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="703" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A703" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B703" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C703" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D703" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E703" s="3">
+        <v>3</v>
+      </c>
+      <c r="F703" s="3">
+        <v>3.9937999999999998</v>
+      </c>
+      <c r="G703" s="3">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="704" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A704" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B704" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C704" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D704" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E704" s="3">
+        <v>3</v>
+      </c>
+      <c r="F704" s="3">
+        <v>3.9735</v>
+      </c>
+      <c r="G704" s="3">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="705" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A705" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B705" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C705" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D705" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E705" s="3">
+        <v>3</v>
+      </c>
+      <c r="F705" s="3">
+        <v>3.9571000000000001</v>
+      </c>
+      <c r="G705" s="3">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="706" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A706" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B706" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C706" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D706" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E706" s="3">
+        <v>3</v>
+      </c>
+      <c r="F706" s="3">
+        <v>3.9449999999999998</v>
+      </c>
+      <c r="G706" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="707" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A707" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B707" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C707" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D707" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E707" s="3">
+        <v>3</v>
+      </c>
+      <c r="F707" s="3">
+        <v>3.9062999999999999</v>
+      </c>
+      <c r="G707" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="708" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A708" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B708" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C708" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D708" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E708" s="3">
+        <v>3</v>
+      </c>
+      <c r="F708" s="3">
+        <v>3.8473000000000002</v>
+      </c>
+      <c r="G708" s="3">
+        <v>13.9</v>
+      </c>
+    </row>
+    <row r="709" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A709" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B709" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C709" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D709" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E709" s="3">
+        <v>4</v>
+      </c>
+      <c r="F709" s="3">
+        <v>1.8837999999999999</v>
+      </c>
+      <c r="G709" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="710" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A710" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B710" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C710" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D710" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E710" s="3">
+        <v>4</v>
+      </c>
+      <c r="F710" s="3">
+        <v>1.8691</v>
+      </c>
+      <c r="G710" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="711" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A711" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B711" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C711" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D711" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E711" s="3">
+        <v>4</v>
+      </c>
+      <c r="F711" s="3">
+        <v>1.8625</v>
+      </c>
+      <c r="G711" s="3">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="712" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A712" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B712" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C712" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D712" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E712" s="3">
+        <v>4</v>
+      </c>
+      <c r="F712" s="3">
+        <v>1.8562000000000001</v>
+      </c>
+      <c r="G712" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="713" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A713" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B713" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C713" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D713" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E713" s="3">
+        <v>4</v>
+      </c>
+      <c r="F713" s="3">
+        <v>1.8502000000000001</v>
+      </c>
+      <c r="G713" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="714" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A714" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B714" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C714" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D714" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E714" s="3">
+        <v>4</v>
+      </c>
+      <c r="F714" s="3">
+        <v>1.8127</v>
+      </c>
+      <c r="G714" s="3">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="715" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A715" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B715" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C715" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D715" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E715" s="3">
+        <v>4</v>
+      </c>
+      <c r="F715" s="3">
+        <v>1.7844</v>
+      </c>
+      <c r="G715" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="716" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A716" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B716" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C716" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D716" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E716" s="3">
+        <v>4</v>
+      </c>
+      <c r="F716" s="3">
+        <v>1.6883999999999999</v>
+      </c>
+      <c r="G716" s="3">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="717" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A717" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B717" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C717" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D717" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E717" s="3">
+        <v>5</v>
+      </c>
+      <c r="F717" s="3">
+        <v>1.4443999999999999</v>
+      </c>
+      <c r="G717" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="718" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A718" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B718" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C718" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D718" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E718" s="3">
+        <v>5</v>
+      </c>
+      <c r="F718" s="3">
+        <v>1.4046000000000001</v>
+      </c>
+      <c r="G718" s="3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="719" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A719" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B719" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C719" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D719" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E719" s="3">
+        <v>5</v>
+      </c>
+      <c r="F719" s="3">
+        <v>1.3775999999999999</v>
+      </c>
+      <c r="G719" s="3">
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="720" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A720" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B720" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C720" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D720" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E720" s="3">
+        <v>5</v>
+      </c>
+      <c r="F720" s="3">
+        <v>1.3513999999999999</v>
+      </c>
+      <c r="G720" s="3">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="721" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A721" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B721" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C721" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D721" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E721" s="3">
+        <v>5</v>
+      </c>
+      <c r="F721" s="3">
+        <v>1.2968999999999999</v>
+      </c>
+      <c r="G721" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="722" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A722" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B722" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C722" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D722" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E722" s="3">
+        <v>5</v>
+      </c>
+      <c r="F722" s="3">
+        <v>1.2763</v>
+      </c>
+      <c r="G722" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="723" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A723" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B723" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C723" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D723" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E723" s="3">
+        <v>5</v>
+      </c>
+      <c r="F723" s="3">
+        <v>1.2521</v>
+      </c>
+      <c r="G723" s="3">
+        <v>13.6</v>
+      </c>
+    </row>
+    <row r="724" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A724" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B724" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C724" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D724" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E724" s="3">
+        <v>5</v>
+      </c>
+      <c r="F724" s="3">
+        <v>1.2172000000000001</v>
+      </c>
+      <c r="G724" s="3">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="725" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A725" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B725" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C725" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D725" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E725" s="3">
+        <v>5</v>
+      </c>
+      <c r="F725" s="3">
+        <v>1.1617999999999999</v>
+      </c>
+      <c r="G725" s="3">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="726" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A726" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B726" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C726" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D726" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E726" s="3">
+        <v>6</v>
+      </c>
+      <c r="F726" s="3">
+        <v>1.23</v>
+      </c>
+      <c r="G726" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="727" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A727" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B727" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C727" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D727" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E727" s="3">
+        <v>6</v>
+      </c>
+      <c r="F727" s="3">
+        <v>1.2170000000000001</v>
+      </c>
+      <c r="G727" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="728" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A728" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B728" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C728" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D728" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E728" s="3">
+        <v>6</v>
+      </c>
+      <c r="F728" s="3">
+        <v>1.2128000000000001</v>
+      </c>
+      <c r="G728" s="3">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="729" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A729" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B729" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C729" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D729" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E729" s="3">
+        <v>6</v>
+      </c>
+      <c r="F729" s="3">
+        <v>1.2091000000000001</v>
+      </c>
+      <c r="G729" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="730" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A730" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B730" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C730" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D730" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E730" s="3">
+        <v>6</v>
+      </c>
+      <c r="F730" s="3">
+        <v>1.2049000000000001</v>
+      </c>
+      <c r="G730" s="3">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="731" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A731" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B731" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C731" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D731" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E731" s="3">
+        <v>6</v>
+      </c>
+      <c r="F731" s="3">
+        <v>1.1991000000000001</v>
+      </c>
+      <c r="G731" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="732" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A732" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B732" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C732" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D732" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E732" s="3">
+        <v>6</v>
+      </c>
+      <c r="F732" s="3">
+        <v>1.1944999999999999</v>
+      </c>
+      <c r="G732" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="733" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A733" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B733" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C733" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D733" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E733" s="3">
+        <v>6</v>
+      </c>
+      <c r="F733" s="3">
+        <v>1.1909000000000001</v>
+      </c>
+      <c r="G733" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="734" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A734" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B734" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C734" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D734" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E734" s="3">
+        <v>6</v>
+      </c>
+      <c r="F734" s="3">
+        <v>1.1861999999999999</v>
+      </c>
+      <c r="G734" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="735" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A735" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B735" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C735" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D735" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E735" s="3">
+        <v>6</v>
+      </c>
+      <c r="F735" s="3">
+        <v>1.1587000000000001</v>
+      </c>
+      <c r="G735" s="3">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="736" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A736" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B736" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C736" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D736" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E736" s="3">
+        <v>6</v>
+      </c>
+      <c r="F736" s="3">
+        <v>1.1501999999999999</v>
+      </c>
+      <c r="G736" s="3">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="737" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A737" t="s">
+        <v>5</v>
+      </c>
+      <c r="B737" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C737" t="s">
+        <v>32</v>
+      </c>
+      <c r="D737" t="s">
+        <v>11</v>
+      </c>
+      <c r="E737">
+        <v>2</v>
+      </c>
+      <c r="F737" s="3">
+        <v>1.1899299999999999</v>
+      </c>
+      <c r="G737" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="738" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A738" t="s">
+        <v>5</v>
+      </c>
+      <c r="B738" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C738" t="s">
+        <v>32</v>
+      </c>
+      <c r="D738" t="s">
+        <v>11</v>
+      </c>
+      <c r="E738">
+        <v>2</v>
+      </c>
+      <c r="F738" s="3">
+        <v>1.8777999999999999</v>
+      </c>
+      <c r="G738" s="3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="739" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A739" t="s">
+        <v>5</v>
+      </c>
+      <c r="B739" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C739" t="s">
+        <v>32</v>
+      </c>
+      <c r="D739" t="s">
+        <v>11</v>
+      </c>
+      <c r="E739">
+        <v>2</v>
+      </c>
+      <c r="F739" s="3">
+        <v>1.8305</v>
+      </c>
+      <c r="G739" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="740" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A740" t="s">
+        <v>5</v>
+      </c>
+      <c r="B740" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C740" t="s">
+        <v>32</v>
+      </c>
+      <c r="D740" t="s">
+        <v>11</v>
+      </c>
+      <c r="E740">
+        <v>2</v>
+      </c>
+      <c r="F740" s="3">
+        <v>1.7944</v>
+      </c>
+      <c r="G740" s="3">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="741" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A741" t="s">
+        <v>5</v>
+      </c>
+      <c r="B741" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C741" t="s">
+        <v>32</v>
+      </c>
+      <c r="D741" t="s">
+        <v>11</v>
+      </c>
+      <c r="E741">
+        <v>2</v>
+      </c>
+      <c r="F741" s="3">
+        <v>1.7594000000000001</v>
+      </c>
+      <c r="G741" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="742" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A742" t="s">
+        <v>5</v>
+      </c>
+      <c r="B742" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C742" t="s">
+        <v>32</v>
+      </c>
+      <c r="D742" t="s">
+        <v>11</v>
+      </c>
+      <c r="E742">
+        <v>2</v>
+      </c>
+      <c r="F742" s="3">
+        <v>1.7366999999999999</v>
+      </c>
+      <c r="G742" s="3">
+        <v>8.6999999999999993</v>
+      </c>
+    </row>
+    <row r="743" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A743" t="s">
+        <v>5</v>
+      </c>
+      <c r="B743" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C743" t="s">
+        <v>32</v>
+      </c>
+      <c r="D743" t="s">
+        <v>11</v>
+      </c>
+      <c r="E743">
+        <v>2</v>
+      </c>
+      <c r="F743" s="3">
+        <v>1.7103999999999999</v>
+      </c>
+      <c r="G743" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="744" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A744" t="s">
+        <v>5</v>
+      </c>
+      <c r="B744" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C744" t="s">
+        <v>32</v>
+      </c>
+      <c r="D744" t="s">
+        <v>11</v>
+      </c>
+      <c r="E744">
+        <v>2</v>
+      </c>
+      <c r="F744" s="3">
+        <v>1.6929000000000001</v>
+      </c>
+      <c r="G744" s="3">
+        <v>13.8</v>
+      </c>
+    </row>
+    <row r="745" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A745" t="s">
+        <v>5</v>
+      </c>
+      <c r="B745" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C745" t="s">
+        <v>32</v>
+      </c>
+      <c r="D745" t="s">
+        <v>11</v>
+      </c>
+      <c r="E745">
+        <v>2</v>
+      </c>
+      <c r="F745" s="3">
+        <v>1.6563000000000001</v>
+      </c>
+      <c r="G745" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="746" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A746" t="s">
+        <v>5</v>
+      </c>
+      <c r="B746" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C746" t="s">
+        <v>32</v>
+      </c>
+      <c r="D746" t="s">
+        <v>11</v>
+      </c>
+      <c r="E746">
+        <v>2</v>
+      </c>
+      <c r="F746" s="3">
+        <v>1.5820000000000001</v>
+      </c>
+      <c r="G746" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="747" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A747" t="s">
+        <v>5</v>
+      </c>
+      <c r="B747" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C747" t="s">
+        <v>32</v>
+      </c>
+      <c r="D747" t="s">
+        <v>11</v>
+      </c>
+      <c r="E747">
+        <v>3</v>
+      </c>
+      <c r="F747" s="3">
+        <v>1.6458999999999999</v>
+      </c>
+      <c r="G747" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="748" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A748" t="s">
+        <v>5</v>
+      </c>
+      <c r="B748" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C748" t="s">
+        <v>32</v>
+      </c>
+      <c r="D748" t="s">
+        <v>11</v>
+      </c>
+      <c r="E748">
+        <v>3</v>
+      </c>
+      <c r="F748" s="3">
+        <v>1.6180000000000001</v>
+      </c>
+      <c r="G748" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="749" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A749" t="s">
+        <v>5</v>
+      </c>
+      <c r="B749" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C749" t="s">
+        <v>32</v>
+      </c>
+      <c r="D749" t="s">
+        <v>11</v>
+      </c>
+      <c r="E749">
+        <v>3</v>
+      </c>
+      <c r="F749" s="3">
+        <v>1.6027</v>
+      </c>
+      <c r="G749" s="3">
+        <v>6.9</v>
+      </c>
+    </row>
+    <row r="750" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A750" t="s">
+        <v>5</v>
+      </c>
+      <c r="B750" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C750" t="s">
+        <v>32</v>
+      </c>
+      <c r="D750" t="s">
+        <v>11</v>
+      </c>
+      <c r="E750">
+        <v>3</v>
+      </c>
+      <c r="F750" s="3">
+        <v>1.5913999999999999</v>
+      </c>
+      <c r="G750" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="751" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A751" t="s">
+        <v>5</v>
+      </c>
+      <c r="B751" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C751" t="s">
+        <v>32</v>
+      </c>
+      <c r="D751" t="s">
+        <v>11</v>
+      </c>
+      <c r="E751">
+        <v>3</v>
+      </c>
+      <c r="F751" s="3">
+        <v>1.5812999999999999</v>
+      </c>
+      <c r="G751" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="752" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A752" t="s">
+        <v>5</v>
+      </c>
+      <c r="B752" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C752" t="s">
+        <v>32</v>
+      </c>
+      <c r="D752" t="s">
+        <v>11</v>
+      </c>
+      <c r="E752">
+        <v>3</v>
+      </c>
+      <c r="F752" s="3">
+        <v>1.5667</v>
+      </c>
+      <c r="G752" s="3">
+        <v>11.2</v>
+      </c>
+    </row>
+    <row r="753" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A753" t="s">
+        <v>5</v>
+      </c>
+      <c r="B753" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C753" t="s">
+        <v>32</v>
+      </c>
+      <c r="D753" t="s">
+        <v>11</v>
+      </c>
+      <c r="E753">
+        <v>3</v>
+      </c>
+      <c r="F753" s="3">
+        <v>1.5359</v>
+      </c>
+      <c r="G753" s="3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="754" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A754" t="s">
+        <v>5</v>
+      </c>
+      <c r="B754" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C754" t="s">
+        <v>32</v>
+      </c>
+      <c r="D754" t="s">
+        <v>11</v>
+      </c>
+      <c r="E754">
+        <v>3</v>
+      </c>
+      <c r="F754" s="3">
+        <v>1.5019</v>
+      </c>
+      <c r="G754" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="755" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A755" t="s">
+        <v>5</v>
+      </c>
+      <c r="B755" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C755" t="s">
+        <v>32</v>
+      </c>
+      <c r="D755" t="s">
+        <v>11</v>
+      </c>
+      <c r="E755">
+        <v>3</v>
+      </c>
+      <c r="F755" s="3">
+        <v>1.4716</v>
+      </c>
+      <c r="G755" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="756" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A756" t="s">
+        <v>5</v>
+      </c>
+      <c r="B756" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C756" t="s">
+        <v>32</v>
+      </c>
+      <c r="D756" t="s">
+        <v>11</v>
+      </c>
+      <c r="E756">
+        <v>4</v>
+      </c>
+      <c r="F756" s="3">
+        <v>2.2128999999999999</v>
+      </c>
+      <c r="G756" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="757" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A757" t="s">
+        <v>5</v>
+      </c>
+      <c r="B757" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C757" t="s">
+        <v>32</v>
+      </c>
+      <c r="D757" t="s">
+        <v>11</v>
+      </c>
+      <c r="E757">
+        <v>4</v>
+      </c>
+      <c r="F757" s="3">
+        <v>2.1634000000000002</v>
+      </c>
+      <c r="G757" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="758" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A758" t="s">
+        <v>5</v>
+      </c>
+      <c r="B758" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C758" t="s">
+        <v>32</v>
+      </c>
+      <c r="D758" t="s">
+        <v>11</v>
+      </c>
+      <c r="E758">
+        <v>4</v>
+      </c>
+      <c r="F758" s="3">
+        <v>2.1377000000000002</v>
+      </c>
+      <c r="G758" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="759" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A759" t="s">
+        <v>5</v>
+      </c>
+      <c r="B759" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C759" t="s">
+        <v>32</v>
+      </c>
+      <c r="D759" t="s">
+        <v>11</v>
+      </c>
+      <c r="E759">
+        <v>4</v>
+      </c>
+      <c r="F759" s="3">
+        <v>2.1257000000000001</v>
+      </c>
+      <c r="G759" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="760" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A760" t="s">
+        <v>5</v>
+      </c>
+      <c r="B760" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C760" t="s">
+        <v>32</v>
+      </c>
+      <c r="D760" t="s">
+        <v>11</v>
+      </c>
+      <c r="E760">
+        <v>4</v>
+      </c>
+      <c r="F760" s="3">
+        <v>2.1149</v>
+      </c>
+      <c r="G760" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="761" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A761" t="s">
+        <v>5</v>
+      </c>
+      <c r="B761" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C761" t="s">
+        <v>32</v>
+      </c>
+      <c r="D761" t="s">
+        <v>11</v>
+      </c>
+      <c r="E761">
+        <v>4</v>
+      </c>
+      <c r="F761" s="3">
+        <v>2.1034000000000002</v>
+      </c>
+      <c r="G761" s="3">
+        <v>11.7</v>
+      </c>
+    </row>
+    <row r="762" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A762" t="s">
+        <v>5</v>
+      </c>
+      <c r="B762" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C762" t="s">
+        <v>32</v>
+      </c>
+      <c r="D762" t="s">
+        <v>11</v>
+      </c>
+      <c r="E762">
+        <v>4</v>
+      </c>
+      <c r="F762" s="3">
+        <v>2.0924</v>
+      </c>
+      <c r="G762" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="763" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A763" t="s">
+        <v>5</v>
+      </c>
+      <c r="B763" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C763" t="s">
+        <v>32</v>
+      </c>
+      <c r="D763" t="s">
+        <v>11</v>
+      </c>
+      <c r="E763">
+        <v>4</v>
+      </c>
+      <c r="F763" s="3">
+        <v>2.0783999999999998</v>
+      </c>
+      <c r="G763" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="764" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A764" t="s">
+        <v>5</v>
+      </c>
+      <c r="B764" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C764" t="s">
+        <v>32</v>
+      </c>
+      <c r="D764" t="s">
+        <v>11</v>
+      </c>
+      <c r="E764">
+        <v>4</v>
+      </c>
+      <c r="F764" s="3">
+        <v>2.0404</v>
+      </c>
+      <c r="G764" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="765" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A765" t="s">
+        <v>5</v>
+      </c>
+      <c r="B765" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C765" t="s">
+        <v>32</v>
+      </c>
+      <c r="D765" t="s">
+        <v>11</v>
+      </c>
+      <c r="E765">
+        <v>4</v>
+      </c>
+      <c r="F765" s="3">
+        <v>1.9763999999999999</v>
+      </c>
+      <c r="G765" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="766" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A766" t="s">
+        <v>5</v>
+      </c>
+      <c r="B766" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C766" t="s">
+        <v>32</v>
+      </c>
+      <c r="D766" t="s">
+        <v>11</v>
+      </c>
+      <c r="E766">
+        <v>4</v>
+      </c>
+      <c r="F766" s="3">
+        <v>1.9027000000000001</v>
+      </c>
+      <c r="G766" s="3">
+        <v>16.100000000000001</v>
+      </c>
+    </row>
+    <row r="767" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A767" t="s">
+        <v>5</v>
+      </c>
+      <c r="B767" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C767" t="s">
+        <v>32</v>
+      </c>
+      <c r="D767" t="s">
+        <v>11</v>
+      </c>
+      <c r="E767">
+        <v>6</v>
+      </c>
+      <c r="F767" s="3">
+        <v>1.7585999999999999</v>
+      </c>
+      <c r="G767" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="768" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A768" t="s">
+        <v>5</v>
+      </c>
+      <c r="B768" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C768" t="s">
+        <v>32</v>
+      </c>
+      <c r="D768" t="s">
+        <v>11</v>
+      </c>
+      <c r="E768">
+        <v>6</v>
+      </c>
+      <c r="F768" s="3">
+        <v>1.7434000000000001</v>
+      </c>
+      <c r="G768" s="3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="769" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A769" t="s">
+        <v>5</v>
+      </c>
+      <c r="B769" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C769" t="s">
+        <v>32</v>
+      </c>
+      <c r="D769" t="s">
+        <v>11</v>
+      </c>
+      <c r="E769">
+        <v>6</v>
+      </c>
+      <c r="F769" s="3">
+        <v>1.7363</v>
+      </c>
+      <c r="G769" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="770" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A770" t="s">
+        <v>5</v>
+      </c>
+      <c r="B770" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C770" t="s">
+        <v>32</v>
+      </c>
+      <c r="D770" t="s">
+        <v>11</v>
+      </c>
+      <c r="E770">
+        <v>6</v>
+      </c>
+      <c r="F770" s="3">
+        <v>1.7265999999999999</v>
+      </c>
+      <c r="G770" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="771" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A771" t="s">
+        <v>5</v>
+      </c>
+      <c r="B771" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C771" t="s">
+        <v>32</v>
+      </c>
+      <c r="D771" t="s">
+        <v>11</v>
+      </c>
+      <c r="E771">
+        <v>6</v>
+      </c>
+      <c r="F771" s="3">
+        <v>1.7164999999999999</v>
+      </c>
+      <c r="G771" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="772" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A772" t="s">
+        <v>5</v>
+      </c>
+      <c r="B772" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C772" t="s">
+        <v>32</v>
+      </c>
+      <c r="D772" t="s">
+        <v>11</v>
+      </c>
+      <c r="E772">
+        <v>6</v>
+      </c>
+      <c r="F772" s="3">
+        <v>1.7065999999999999</v>
+      </c>
+      <c r="G772" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="773" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A773" t="s">
+        <v>5</v>
+      </c>
+      <c r="B773" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C773" t="s">
+        <v>32</v>
+      </c>
+      <c r="D773" t="s">
+        <v>11</v>
+      </c>
+      <c r="E773">
+        <v>6</v>
+      </c>
+      <c r="F773" s="3">
+        <v>1.6970000000000001</v>
+      </c>
+      <c r="G773" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="774" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A774" t="s">
+        <v>5</v>
+      </c>
+      <c r="B774" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C774" t="s">
+        <v>32</v>
+      </c>
+      <c r="D774" t="s">
+        <v>11</v>
+      </c>
+      <c r="E774">
+        <v>6</v>
+      </c>
+      <c r="F774" s="3">
+        <v>1.6667000000000001</v>
+      </c>
+      <c r="G774" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="775" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A775" t="s">
+        <v>5</v>
+      </c>
+      <c r="B775" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C775" t="s">
+        <v>32</v>
+      </c>
+      <c r="D775" t="s">
+        <v>11</v>
+      </c>
+      <c r="E775">
+        <v>6</v>
+      </c>
+      <c r="F775" s="3">
+        <v>1.6326000000000001</v>
+      </c>
+      <c r="G775" s="3">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="776" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A776" t="s">
+        <v>5</v>
+      </c>
+      <c r="B776" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C776" t="s">
+        <v>32</v>
+      </c>
+      <c r="D776" t="s">
+        <v>11</v>
+      </c>
+      <c r="E776">
+        <v>6</v>
+      </c>
+      <c r="F776" s="3">
+        <v>1.5609</v>
+      </c>
+      <c r="G776" s="3">
+        <v>11.3</v>
+      </c>
+    </row>
+    <row r="777" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A777" t="s">
+        <v>5</v>
+      </c>
+      <c r="B777" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C777" t="s">
+        <v>32</v>
+      </c>
+      <c r="D777" t="s">
+        <v>11</v>
+      </c>
+      <c r="E777">
+        <v>6</v>
+      </c>
+      <c r="F777" s="3">
+        <v>1.5167999999999999</v>
+      </c>
+      <c r="G777" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="778" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A778" t="s">
+        <v>5</v>
+      </c>
+      <c r="B778" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C778" t="s">
+        <v>32</v>
+      </c>
+      <c r="D778" t="s">
+        <v>11</v>
+      </c>
+      <c r="E778">
+        <v>6</v>
+      </c>
+      <c r="F778" s="3">
+        <v>1.5049999999999999</v>
+      </c>
+      <c r="G778" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="779" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A779" t="s">
+        <v>5</v>
+      </c>
+      <c r="B779" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C779" t="s">
+        <v>32</v>
+      </c>
+      <c r="D779" t="s">
+        <v>11</v>
+      </c>
+      <c r="E779">
+        <v>7</v>
+      </c>
+      <c r="F779" s="3">
+        <v>1.3242</v>
+      </c>
+      <c r="G779" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="780" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A780" t="s">
+        <v>5</v>
+      </c>
+      <c r="B780" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C780" t="s">
+        <v>32</v>
+      </c>
+      <c r="D780" t="s">
+        <v>11</v>
+      </c>
+      <c r="E780">
+        <v>7</v>
+      </c>
+      <c r="F780" s="3">
+        <v>1.3148</v>
+      </c>
+      <c r="G780" s="3">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="781" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A781" t="s">
+        <v>5</v>
+      </c>
+      <c r="B781" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C781" t="s">
+        <v>32</v>
+      </c>
+      <c r="D781" t="s">
+        <v>11</v>
+      </c>
+      <c r="E781">
+        <v>7</v>
+      </c>
+      <c r="F781" s="3">
+        <v>1.3010999999999999</v>
+      </c>
+      <c r="G781" s="3">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="782" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A782" t="s">
+        <v>5</v>
+      </c>
+      <c r="B782" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C782" t="s">
+        <v>32</v>
+      </c>
+      <c r="D782" t="s">
+        <v>11</v>
+      </c>
+      <c r="E782">
+        <v>7</v>
+      </c>
+      <c r="F782" s="3">
+        <v>1.2928999999999999</v>
+      </c>
+      <c r="G782" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="783" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A783" t="s">
+        <v>5</v>
+      </c>
+      <c r="B783" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C783" t="s">
+        <v>32</v>
+      </c>
+      <c r="D783" t="s">
+        <v>11</v>
+      </c>
+      <c r="E783">
+        <v>7</v>
+      </c>
+      <c r="F783" s="3">
+        <v>1.2857000000000001</v>
+      </c>
+      <c r="G783" s="3">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="784" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A784" t="s">
+        <v>5</v>
+      </c>
+      <c r="B784" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C784" t="s">
+        <v>32</v>
+      </c>
+      <c r="D784" t="s">
+        <v>11</v>
+      </c>
+      <c r="E784">
+        <v>7</v>
+      </c>
+      <c r="F784" s="3">
+        <v>1.2703</v>
+      </c>
+      <c r="G784" s="3">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="785" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A785" t="s">
+        <v>5</v>
+      </c>
+      <c r="B785" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C785" t="s">
+        <v>32</v>
+      </c>
+      <c r="D785" t="s">
+        <v>11</v>
+      </c>
+      <c r="E785">
+        <v>7</v>
+      </c>
+      <c r="F785" s="3">
+        <v>1.2478</v>
+      </c>
+      <c r="G785" s="3">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="786" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A786" t="s">
+        <v>5</v>
+      </c>
+      <c r="B786" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C786" t="s">
+        <v>32</v>
+      </c>
+      <c r="D786" t="s">
+        <v>11</v>
+      </c>
+      <c r="E786">
+        <v>7</v>
+      </c>
+      <c r="F786" s="3">
+        <v>1.1932</v>
+      </c>
+      <c r="G786" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="787" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A787" t="s">
+        <v>5</v>
+      </c>
+      <c r="B787" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C787" t="s">
+        <v>32</v>
+      </c>
+      <c r="D787" t="s">
+        <v>11</v>
+      </c>
+      <c r="E787">
+        <v>8</v>
+      </c>
+      <c r="F787" s="3">
+        <v>1.4159999999999999</v>
+      </c>
+      <c r="G787" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="788" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A788" t="s">
+        <v>5</v>
+      </c>
+      <c r="B788" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C788" t="s">
+        <v>32</v>
+      </c>
+      <c r="D788" t="s">
+        <v>11</v>
+      </c>
+      <c r="E788">
+        <v>8</v>
+      </c>
+      <c r="F788" s="3">
+        <v>1.4025000000000001</v>
+      </c>
+      <c r="G788" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="789" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A789" t="s">
+        <v>5</v>
+      </c>
+      <c r="B789" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C789" t="s">
+        <v>32</v>
+      </c>
+      <c r="D789" t="s">
+        <v>11</v>
+      </c>
+      <c r="E789">
+        <v>8</v>
+      </c>
+      <c r="F789" s="3">
+        <v>4.3933</v>
+      </c>
+      <c r="G789" s="3">
+        <v>5.3</v>
+      </c>
+    </row>
+    <row r="790" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A790" t="s">
+        <v>5</v>
+      </c>
+      <c r="B790" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C790" t="s">
+        <v>32</v>
+      </c>
+      <c r="D790" t="s">
+        <v>11</v>
+      </c>
+      <c r="E790">
+        <v>8</v>
+      </c>
+      <c r="F790" s="3">
+        <v>1.3894</v>
+      </c>
+      <c r="G790" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="791" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A791" t="s">
+        <v>5</v>
+      </c>
+      <c r="B791" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C791" t="s">
+        <v>32</v>
+      </c>
+      <c r="D791" t="s">
+        <v>11</v>
+      </c>
+      <c r="E791">
+        <v>8</v>
+      </c>
+      <c r="F791" s="3">
+        <v>1.3847</v>
+      </c>
+      <c r="G791" s="3">
+        <v>7.3</v>
+      </c>
+    </row>
+    <row r="792" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A792" t="s">
+        <v>5</v>
+      </c>
+      <c r="B792" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C792" t="s">
+        <v>32</v>
+      </c>
+      <c r="D792" t="s">
+        <v>11</v>
+      </c>
+      <c r="E792">
+        <v>8</v>
+      </c>
+      <c r="F792" s="3">
+        <v>1.3749</v>
+      </c>
+      <c r="G792" s="3">
+        <v>8.1</v>
+      </c>
+    </row>
+    <row r="793" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A793" t="s">
+        <v>5</v>
+      </c>
+      <c r="B793" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C793" t="s">
+        <v>32</v>
+      </c>
+      <c r="D793" t="s">
+        <v>11</v>
+      </c>
+      <c r="E793">
+        <v>8</v>
+      </c>
+      <c r="F793" s="3">
+        <v>1.3629</v>
+      </c>
+      <c r="G793" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="794" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A794" t="s">
+        <v>5</v>
+      </c>
+      <c r="B794" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C794" t="s">
+        <v>32</v>
+      </c>
+      <c r="D794" t="s">
+        <v>11</v>
+      </c>
+      <c r="E794">
+        <v>8</v>
+      </c>
+      <c r="F794" s="3">
+        <v>1.349</v>
+      </c>
+      <c r="G794" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="795" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A795" t="s">
+        <v>5</v>
+      </c>
+      <c r="B795" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C795" t="s">
+        <v>32</v>
+      </c>
+      <c r="D795" t="s">
+        <v>11</v>
+      </c>
+      <c r="E795">
+        <v>8</v>
+      </c>
+      <c r="F795" s="3">
+        <v>1.3292999999999999</v>
+      </c>
+      <c r="G795" s="3">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="796" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A796" t="s">
+        <v>5</v>
+      </c>
+      <c r="B796" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C796" t="s">
+        <v>32</v>
+      </c>
+      <c r="D796" t="s">
+        <v>11</v>
+      </c>
+      <c r="E796">
+        <v>8</v>
+      </c>
+      <c r="F796" s="3">
+        <v>1.296</v>
+      </c>
+      <c r="G796" s="3">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="797" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A797" t="s">
+        <v>5</v>
+      </c>
+      <c r="B797" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C797" t="s">
+        <v>32</v>
+      </c>
+      <c r="D797" t="s">
+        <v>11</v>
+      </c>
+      <c r="E797">
+        <v>8</v>
+      </c>
+      <c r="F797" s="3">
+        <v>1.2696000000000001</v>
+      </c>
+      <c r="G797" s="3">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="810" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A810" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B810" s="2">
+        <v>43015</v>
+      </c>
+      <c r="C810" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D810" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E810" s="3">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
more data entry and leaf age files added
</commit_message>
<xml_diff>
--- a/raw_data/pv_curves.xlsx
+++ b/raw_data/pv_curves.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2772" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3497" uniqueCount="38">
   <si>
     <t>species</t>
   </si>
@@ -126,6 +126,18 @@
   </si>
   <si>
     <t>mickelia_nicotianifolia</t>
+  </si>
+  <si>
+    <t>tectaria_incisa</t>
+  </si>
+  <si>
+    <t>asplenium_serratum</t>
+  </si>
+  <si>
+    <t>14/7/2017</t>
+  </si>
+  <si>
+    <t>thelypteris_nicaraguensis</t>
   </si>
 </sst>
 </file>
@@ -488,11 +500,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P810"/>
+  <dimension ref="A1:P988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A781" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H800" sqref="H800"/>
+      <pane ySplit="1" topLeftCell="A948" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E967" sqref="E967"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20791,21 +20803,4260 @@
         <v>12.9</v>
       </c>
     </row>
-    <row r="810" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A810" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B810" s="2">
-        <v>43015</v>
-      </c>
-      <c r="C810" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D810" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E810" s="3">
+    <row r="798" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A798" t="s">
+        <v>5</v>
+      </c>
+      <c r="B798" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C798" t="s">
+        <v>34</v>
+      </c>
+      <c r="D798" t="s">
+        <v>11</v>
+      </c>
+      <c r="E798">
         <v>1</v>
+      </c>
+      <c r="F798" s="3">
+        <v>2.8321999999999998</v>
+      </c>
+      <c r="G798" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="799" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A799" t="s">
+        <v>5</v>
+      </c>
+      <c r="B799" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C799" t="s">
+        <v>34</v>
+      </c>
+      <c r="D799" t="s">
+        <v>11</v>
+      </c>
+      <c r="E799">
+        <v>1</v>
+      </c>
+      <c r="F799" s="3">
+        <v>2.6488999999999998</v>
+      </c>
+      <c r="G799" s="3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="800" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A800" t="s">
+        <v>5</v>
+      </c>
+      <c r="B800" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C800" t="s">
+        <v>34</v>
+      </c>
+      <c r="D800" t="s">
+        <v>11</v>
+      </c>
+      <c r="E800">
+        <v>1</v>
+      </c>
+      <c r="F800" s="3">
+        <v>2.6023000000000001</v>
+      </c>
+      <c r="G800" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="801" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A801" t="s">
+        <v>5</v>
+      </c>
+      <c r="B801" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C801" t="s">
+        <v>34</v>
+      </c>
+      <c r="D801" t="s">
+        <v>11</v>
+      </c>
+      <c r="E801">
+        <v>1</v>
+      </c>
+      <c r="F801" s="3">
+        <v>2.581</v>
+      </c>
+      <c r="G801" s="3">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="802" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A802" t="s">
+        <v>5</v>
+      </c>
+      <c r="B802" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C802" t="s">
+        <v>34</v>
+      </c>
+      <c r="D802" t="s">
+        <v>11</v>
+      </c>
+      <c r="E802">
+        <v>1</v>
+      </c>
+      <c r="F802" s="3">
+        <v>2.5375999999999999</v>
+      </c>
+      <c r="G802" s="3">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="803" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A803" t="s">
+        <v>5</v>
+      </c>
+      <c r="B803" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C803" t="s">
+        <v>34</v>
+      </c>
+      <c r="D803" t="s">
+        <v>11</v>
+      </c>
+      <c r="E803">
+        <v>1</v>
+      </c>
+      <c r="F803" s="3">
+        <v>2.4710999999999999</v>
+      </c>
+      <c r="G803" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="804" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A804" t="s">
+        <v>5</v>
+      </c>
+      <c r="B804" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C804" t="s">
+        <v>34</v>
+      </c>
+      <c r="D804" t="s">
+        <v>11</v>
+      </c>
+      <c r="E804">
+        <v>1</v>
+      </c>
+      <c r="F804" s="3">
+        <v>2.2746</v>
+      </c>
+      <c r="G804" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="805" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A805" t="s">
+        <v>5</v>
+      </c>
+      <c r="B805" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C805" t="s">
+        <v>34</v>
+      </c>
+      <c r="D805" t="s">
+        <v>11</v>
+      </c>
+      <c r="E805">
+        <v>2</v>
+      </c>
+      <c r="F805" s="3">
+        <v>3.8100999999999998</v>
+      </c>
+      <c r="G805" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="806" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A806" t="s">
+        <v>5</v>
+      </c>
+      <c r="B806" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C806" t="s">
+        <v>34</v>
+      </c>
+      <c r="D806" t="s">
+        <v>11</v>
+      </c>
+      <c r="E806">
+        <v>2</v>
+      </c>
+      <c r="F806" s="3">
+        <v>3.7433000000000001</v>
+      </c>
+      <c r="G806" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="807" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A807" t="s">
+        <v>5</v>
+      </c>
+      <c r="B807" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C807" t="s">
+        <v>34</v>
+      </c>
+      <c r="D807" t="s">
+        <v>11</v>
+      </c>
+      <c r="E807">
+        <v>2</v>
+      </c>
+      <c r="F807" s="3">
+        <v>3.6897000000000002</v>
+      </c>
+      <c r="G807" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="808" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A808" t="s">
+        <v>5</v>
+      </c>
+      <c r="B808" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C808" t="s">
+        <v>34</v>
+      </c>
+      <c r="D808" t="s">
+        <v>11</v>
+      </c>
+      <c r="E808">
+        <v>2</v>
+      </c>
+      <c r="F808" s="3">
+        <v>3.6446000000000001</v>
+      </c>
+      <c r="G808" s="3">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="809" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A809" t="s">
+        <v>5</v>
+      </c>
+      <c r="B809" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C809" t="s">
+        <v>34</v>
+      </c>
+      <c r="D809" t="s">
+        <v>11</v>
+      </c>
+      <c r="E809">
+        <v>2</v>
+      </c>
+      <c r="F809" s="3">
+        <v>3.6073</v>
+      </c>
+      <c r="G809" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="810" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A810" t="s">
+        <v>5</v>
+      </c>
+      <c r="B810" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C810" t="s">
+        <v>34</v>
+      </c>
+      <c r="D810" t="s">
+        <v>11</v>
+      </c>
+      <c r="E810">
+        <v>2</v>
+      </c>
+      <c r="F810" s="3">
+        <v>3.536</v>
+      </c>
+      <c r="G810" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="811" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A811" t="s">
+        <v>5</v>
+      </c>
+      <c r="B811" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C811" t="s">
+        <v>34</v>
+      </c>
+      <c r="D811" t="s">
+        <v>11</v>
+      </c>
+      <c r="E811">
+        <v>2</v>
+      </c>
+      <c r="F811" s="3">
+        <v>3.4622000000000002</v>
+      </c>
+      <c r="G811" s="3">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="812" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A812" t="s">
+        <v>5</v>
+      </c>
+      <c r="B812" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C812" t="s">
+        <v>34</v>
+      </c>
+      <c r="D812" t="s">
+        <v>11</v>
+      </c>
+      <c r="E812">
+        <v>2</v>
+      </c>
+      <c r="F812" s="3">
+        <v>3.2174999999999998</v>
+      </c>
+      <c r="G812" s="3">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="813" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A813" t="s">
+        <v>5</v>
+      </c>
+      <c r="B813" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C813" t="s">
+        <v>34</v>
+      </c>
+      <c r="D813" t="s">
+        <v>11</v>
+      </c>
+      <c r="E813">
+        <v>2</v>
+      </c>
+      <c r="F813" s="3">
+        <v>3.4081999999999999</v>
+      </c>
+      <c r="G813" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="814" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A814" t="s">
+        <v>5</v>
+      </c>
+      <c r="B814" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C814" t="s">
+        <v>34</v>
+      </c>
+      <c r="D814" t="s">
+        <v>11</v>
+      </c>
+      <c r="E814">
+        <v>3</v>
+      </c>
+      <c r="F814" s="3">
+        <v>3.3940000000000001</v>
+      </c>
+      <c r="G814" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="815" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A815" t="s">
+        <v>5</v>
+      </c>
+      <c r="B815" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C815" t="s">
+        <v>34</v>
+      </c>
+      <c r="D815" t="s">
+        <v>11</v>
+      </c>
+      <c r="E815">
+        <v>3</v>
+      </c>
+      <c r="F815" s="3">
+        <v>3.2035</v>
+      </c>
+      <c r="G815" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="816" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A816" t="s">
+        <v>5</v>
+      </c>
+      <c r="B816" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C816" t="s">
+        <v>34</v>
+      </c>
+      <c r="D816" t="s">
+        <v>11</v>
+      </c>
+      <c r="E816">
+        <v>3</v>
+      </c>
+      <c r="F816" s="3">
+        <v>3.1074000000000002</v>
+      </c>
+      <c r="G816" s="3">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="817" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A817" t="s">
+        <v>5</v>
+      </c>
+      <c r="B817" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C817" t="s">
+        <v>34</v>
+      </c>
+      <c r="D817" t="s">
+        <v>11</v>
+      </c>
+      <c r="E817">
+        <v>3</v>
+      </c>
+      <c r="F817" s="3">
+        <v>3.0893999999999999</v>
+      </c>
+      <c r="G817" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="818" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A818" t="s">
+        <v>5</v>
+      </c>
+      <c r="B818" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C818" t="s">
+        <v>34</v>
+      </c>
+      <c r="D818" t="s">
+        <v>11</v>
+      </c>
+      <c r="E818">
+        <v>3</v>
+      </c>
+      <c r="F818" s="3">
+        <v>2.9950000000000001</v>
+      </c>
+      <c r="G818" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="819" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A819" t="s">
+        <v>5</v>
+      </c>
+      <c r="B819" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C819" t="s">
+        <v>34</v>
+      </c>
+      <c r="D819" t="s">
+        <v>11</v>
+      </c>
+      <c r="E819">
+        <v>3</v>
+      </c>
+      <c r="F819" s="3">
+        <v>2.9339</v>
+      </c>
+      <c r="G819" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="820" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A820" t="s">
+        <v>5</v>
+      </c>
+      <c r="B820" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C820" t="s">
+        <v>34</v>
+      </c>
+      <c r="D820" t="s">
+        <v>11</v>
+      </c>
+      <c r="E820">
+        <v>3</v>
+      </c>
+      <c r="F820" s="3">
+        <v>2.8218000000000001</v>
+      </c>
+      <c r="G820" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="821" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A821" t="s">
+        <v>5</v>
+      </c>
+      <c r="B821" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C821" t="s">
+        <v>34</v>
+      </c>
+      <c r="D821" t="s">
+        <v>11</v>
+      </c>
+      <c r="E821">
+        <v>3</v>
+      </c>
+      <c r="F821" s="3">
+        <v>2.6762999999999999</v>
+      </c>
+      <c r="G821" s="3">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="822" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A822" t="s">
+        <v>5</v>
+      </c>
+      <c r="B822" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C822" t="s">
+        <v>34</v>
+      </c>
+      <c r="D822" t="s">
+        <v>11</v>
+      </c>
+      <c r="E822">
+        <v>4</v>
+      </c>
+      <c r="F822" s="3">
+        <v>3.4270999999999998</v>
+      </c>
+      <c r="G822" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="823" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A823" t="s">
+        <v>5</v>
+      </c>
+      <c r="B823" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C823" t="s">
+        <v>34</v>
+      </c>
+      <c r="D823" t="s">
+        <v>11</v>
+      </c>
+      <c r="E823">
+        <v>4</v>
+      </c>
+      <c r="F823" s="3">
+        <v>3.3961000000000001</v>
+      </c>
+      <c r="G823" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="824" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A824" t="s">
+        <v>5</v>
+      </c>
+      <c r="B824" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C824" t="s">
+        <v>34</v>
+      </c>
+      <c r="D824" t="s">
+        <v>11</v>
+      </c>
+      <c r="E824">
+        <v>4</v>
+      </c>
+      <c r="F824" s="3">
+        <v>3.3871000000000002</v>
+      </c>
+      <c r="G824" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="825" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A825" t="s">
+        <v>5</v>
+      </c>
+      <c r="B825" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C825" t="s">
+        <v>34</v>
+      </c>
+      <c r="D825" t="s">
+        <v>11</v>
+      </c>
+      <c r="E825">
+        <v>4</v>
+      </c>
+      <c r="F825" s="3">
+        <v>3.331</v>
+      </c>
+      <c r="G825" s="3">
+        <v>9.1</v>
+      </c>
+    </row>
+    <row r="826" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A826" t="s">
+        <v>5</v>
+      </c>
+      <c r="B826" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C826" t="s">
+        <v>34</v>
+      </c>
+      <c r="D826" t="s">
+        <v>11</v>
+      </c>
+      <c r="E826">
+        <v>4</v>
+      </c>
+      <c r="F826" s="3">
+        <v>3.2974999999999999</v>
+      </c>
+      <c r="G826" s="3">
+        <v>10.1</v>
+      </c>
+    </row>
+    <row r="827" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A827" t="s">
+        <v>5</v>
+      </c>
+      <c r="B827" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C827" t="s">
+        <v>34</v>
+      </c>
+      <c r="D827" t="s">
+        <v>11</v>
+      </c>
+      <c r="E827">
+        <v>4</v>
+      </c>
+      <c r="F827" s="3">
+        <v>3.2694999999999999</v>
+      </c>
+      <c r="G827" s="3">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="828" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A828" t="s">
+        <v>5</v>
+      </c>
+      <c r="B828" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C828" t="s">
+        <v>34</v>
+      </c>
+      <c r="D828" t="s">
+        <v>11</v>
+      </c>
+      <c r="E828">
+        <v>4</v>
+      </c>
+      <c r="F828" s="3">
+        <v>3.2387999999999999</v>
+      </c>
+      <c r="G828" s="3">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="829" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A829" t="s">
+        <v>5</v>
+      </c>
+      <c r="B829" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C829" t="s">
+        <v>34</v>
+      </c>
+      <c r="D829" t="s">
+        <v>11</v>
+      </c>
+      <c r="E829">
+        <v>4</v>
+      </c>
+      <c r="F829" s="3">
+        <v>3.1907000000000001</v>
+      </c>
+      <c r="G829" s="3">
+        <v>10.6</v>
+      </c>
+    </row>
+    <row r="830" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A830" t="s">
+        <v>5</v>
+      </c>
+      <c r="B830" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C830" t="s">
+        <v>34</v>
+      </c>
+      <c r="D830" t="s">
+        <v>11</v>
+      </c>
+      <c r="E830">
+        <v>4</v>
+      </c>
+      <c r="F830" s="3">
+        <v>3.1</v>
+      </c>
+      <c r="G830" s="3">
+        <v>11.4</v>
+      </c>
+    </row>
+    <row r="831" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A831" t="s">
+        <v>5</v>
+      </c>
+      <c r="B831" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C831" t="s">
+        <v>34</v>
+      </c>
+      <c r="D831" t="s">
+        <v>11</v>
+      </c>
+      <c r="E831">
+        <v>4</v>
+      </c>
+      <c r="F831" s="3">
+        <v>2.8180999999999998</v>
+      </c>
+      <c r="G831" s="3">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="832" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A832" t="s">
+        <v>5</v>
+      </c>
+      <c r="B832" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C832" t="s">
+        <v>34</v>
+      </c>
+      <c r="D832" t="s">
+        <v>11</v>
+      </c>
+      <c r="E832">
+        <v>5</v>
+      </c>
+      <c r="F832" s="3">
+        <v>2.8988</v>
+      </c>
+      <c r="G832" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="833" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A833" t="s">
+        <v>5</v>
+      </c>
+      <c r="B833" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C833" t="s">
+        <v>34</v>
+      </c>
+      <c r="D833" t="s">
+        <v>11</v>
+      </c>
+      <c r="E833">
+        <v>5</v>
+      </c>
+      <c r="F833" s="3">
+        <v>2.8736999999999999</v>
+      </c>
+      <c r="G833" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="834" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A834" t="s">
+        <v>5</v>
+      </c>
+      <c r="B834" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C834" t="s">
+        <v>34</v>
+      </c>
+      <c r="D834" t="s">
+        <v>11</v>
+      </c>
+      <c r="E834">
+        <v>5</v>
+      </c>
+      <c r="F834" s="3">
+        <v>2.8395000000000001</v>
+      </c>
+      <c r="G834" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="835" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A835" t="s">
+        <v>5</v>
+      </c>
+      <c r="B835" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C835" t="s">
+        <v>34</v>
+      </c>
+      <c r="D835" t="s">
+        <v>11</v>
+      </c>
+      <c r="E835">
+        <v>5</v>
+      </c>
+      <c r="F835" s="3">
+        <v>2.8127</v>
+      </c>
+      <c r="G835" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="836" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A836" t="s">
+        <v>5</v>
+      </c>
+      <c r="B836" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C836" t="s">
+        <v>34</v>
+      </c>
+      <c r="D836" t="s">
+        <v>11</v>
+      </c>
+      <c r="E836">
+        <v>5</v>
+      </c>
+      <c r="F836" s="3">
+        <v>2.7719</v>
+      </c>
+      <c r="G836" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="837" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A837" t="s">
+        <v>5</v>
+      </c>
+      <c r="B837" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C837" t="s">
+        <v>34</v>
+      </c>
+      <c r="D837" t="s">
+        <v>11</v>
+      </c>
+      <c r="E837">
+        <v>5</v>
+      </c>
+      <c r="F837" s="3">
+        <v>2.7271000000000001</v>
+      </c>
+      <c r="G837" s="3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="838" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A838" t="s">
+        <v>5</v>
+      </c>
+      <c r="B838" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C838" t="s">
+        <v>34</v>
+      </c>
+      <c r="D838" t="s">
+        <v>11</v>
+      </c>
+      <c r="E838">
+        <v>5</v>
+      </c>
+      <c r="F838" s="3">
+        <v>2.6743000000000001</v>
+      </c>
+      <c r="G838" s="3">
+        <v>9.1999999999999993</v>
+      </c>
+    </row>
+    <row r="839" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A839" t="s">
+        <v>5</v>
+      </c>
+      <c r="B839" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C839" t="s">
+        <v>34</v>
+      </c>
+      <c r="D839" t="s">
+        <v>11</v>
+      </c>
+      <c r="E839">
+        <v>5</v>
+      </c>
+      <c r="F839" s="3">
+        <v>2.4157999999999999</v>
+      </c>
+      <c r="G839" s="3">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="840" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A840" t="s">
+        <v>5</v>
+      </c>
+      <c r="B840" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C840" t="s">
+        <v>34</v>
+      </c>
+      <c r="D840" t="s">
+        <v>11</v>
+      </c>
+      <c r="E840">
+        <v>5</v>
+      </c>
+      <c r="F840" s="3">
+        <v>2.032</v>
+      </c>
+      <c r="G840" s="3">
+        <v>10.9</v>
+      </c>
+    </row>
+    <row r="841" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A841" t="s">
+        <v>5</v>
+      </c>
+      <c r="B841" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C841" t="s">
+        <v>34</v>
+      </c>
+      <c r="D841" t="s">
+        <v>11</v>
+      </c>
+      <c r="E841">
+        <v>6</v>
+      </c>
+      <c r="F841" s="3">
+        <v>3.59</v>
+      </c>
+      <c r="G841" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="842" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A842" t="s">
+        <v>5</v>
+      </c>
+      <c r="B842" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C842" t="s">
+        <v>34</v>
+      </c>
+      <c r="D842" t="s">
+        <v>11</v>
+      </c>
+      <c r="E842">
+        <v>6</v>
+      </c>
+      <c r="F842" s="3">
+        <v>3.5156999999999998</v>
+      </c>
+      <c r="G842" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="843" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A843" t="s">
+        <v>5</v>
+      </c>
+      <c r="B843" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C843" t="s">
+        <v>34</v>
+      </c>
+      <c r="D843" t="s">
+        <v>11</v>
+      </c>
+      <c r="E843">
+        <v>6</v>
+      </c>
+      <c r="F843" s="3">
+        <v>3.4603000000000002</v>
+      </c>
+      <c r="G843" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="844" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A844" t="s">
+        <v>5</v>
+      </c>
+      <c r="B844" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C844" t="s">
+        <v>34</v>
+      </c>
+      <c r="D844" t="s">
+        <v>11</v>
+      </c>
+      <c r="E844">
+        <v>6</v>
+      </c>
+      <c r="F844" s="3">
+        <v>3.4373</v>
+      </c>
+      <c r="G844" s="3">
+        <v>4.9000000000000004</v>
+      </c>
+    </row>
+    <row r="845" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A845" t="s">
+        <v>5</v>
+      </c>
+      <c r="B845" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C845" t="s">
+        <v>34</v>
+      </c>
+      <c r="D845" t="s">
+        <v>11</v>
+      </c>
+      <c r="E845">
+        <v>6</v>
+      </c>
+      <c r="F845" s="3">
+        <v>3.4201999999999999</v>
+      </c>
+      <c r="G845" s="3">
+        <v>6.3</v>
+      </c>
+    </row>
+    <row r="846" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A846" t="s">
+        <v>5</v>
+      </c>
+      <c r="B846" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C846" t="s">
+        <v>34</v>
+      </c>
+      <c r="D846" t="s">
+        <v>11</v>
+      </c>
+      <c r="E846">
+        <v>6</v>
+      </c>
+      <c r="F846" s="3">
+        <v>3.3934000000000002</v>
+      </c>
+      <c r="G846" s="3">
+        <v>7.1</v>
+      </c>
+    </row>
+    <row r="847" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A847" t="s">
+        <v>5</v>
+      </c>
+      <c r="B847" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C847" t="s">
+        <v>34</v>
+      </c>
+      <c r="D847" t="s">
+        <v>11</v>
+      </c>
+      <c r="E847">
+        <v>6</v>
+      </c>
+      <c r="F847" s="3">
+        <v>3.3714</v>
+      </c>
+      <c r="G847" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="848" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A848" t="s">
+        <v>5</v>
+      </c>
+      <c r="B848" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C848" t="s">
+        <v>34</v>
+      </c>
+      <c r="D848" t="s">
+        <v>11</v>
+      </c>
+      <c r="E848">
+        <v>6</v>
+      </c>
+      <c r="F848" s="3">
+        <v>3.2915999999999999</v>
+      </c>
+      <c r="G848" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="849" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A849" t="s">
+        <v>5</v>
+      </c>
+      <c r="B849" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C849" t="s">
+        <v>34</v>
+      </c>
+      <c r="D849" t="s">
+        <v>11</v>
+      </c>
+      <c r="E849">
+        <v>6</v>
+      </c>
+      <c r="F849" s="3">
+        <v>3.2593999999999999</v>
+      </c>
+      <c r="G849" s="3">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="850" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A850" t="s">
+        <v>5</v>
+      </c>
+      <c r="B850" s="4">
+        <v>43016</v>
+      </c>
+      <c r="C850" t="s">
+        <v>34</v>
+      </c>
+      <c r="D850" t="s">
+        <v>11</v>
+      </c>
+      <c r="E850">
+        <v>6</v>
+      </c>
+      <c r="F850" s="3">
+        <v>3.1947000000000001</v>
+      </c>
+      <c r="G850" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="851" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A851" t="s">
+        <v>5</v>
+      </c>
+      <c r="B851" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C851" t="s">
+        <v>35</v>
+      </c>
+      <c r="D851" t="s">
+        <v>6</v>
+      </c>
+      <c r="E851">
+        <v>1</v>
+      </c>
+      <c r="F851" s="3">
+        <v>3.0426000000000002</v>
+      </c>
+      <c r="G851" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="852" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A852" t="s">
+        <v>5</v>
+      </c>
+      <c r="B852" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C852" t="s">
+        <v>35</v>
+      </c>
+      <c r="D852" t="s">
+        <v>6</v>
+      </c>
+      <c r="E852">
+        <v>1</v>
+      </c>
+      <c r="F852" s="3">
+        <v>3.024</v>
+      </c>
+      <c r="G852" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="853" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A853" t="s">
+        <v>5</v>
+      </c>
+      <c r="B853" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C853" t="s">
+        <v>35</v>
+      </c>
+      <c r="D853" t="s">
+        <v>6</v>
+      </c>
+      <c r="E853">
+        <v>1</v>
+      </c>
+      <c r="F853" s="3">
+        <v>3.0103</v>
+      </c>
+      <c r="G853" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="854" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A854" t="s">
+        <v>5</v>
+      </c>
+      <c r="B854" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C854" t="s">
+        <v>35</v>
+      </c>
+      <c r="D854" t="s">
+        <v>6</v>
+      </c>
+      <c r="E854">
+        <v>1</v>
+      </c>
+      <c r="F854" s="3">
+        <v>2.9942000000000002</v>
+      </c>
+      <c r="G854" s="3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="855" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A855" t="s">
+        <v>5</v>
+      </c>
+      <c r="B855" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C855" t="s">
+        <v>35</v>
+      </c>
+      <c r="D855" t="s">
+        <v>6</v>
+      </c>
+      <c r="E855">
+        <v>1</v>
+      </c>
+      <c r="F855" s="3">
+        <v>2.9786000000000001</v>
+      </c>
+      <c r="G855" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="856" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A856" t="s">
+        <v>5</v>
+      </c>
+      <c r="B856" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C856" t="s">
+        <v>35</v>
+      </c>
+      <c r="D856" t="s">
+        <v>6</v>
+      </c>
+      <c r="E856">
+        <v>1</v>
+      </c>
+      <c r="F856" s="3">
+        <v>2.9647999999999999</v>
+      </c>
+      <c r="G856" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="857" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A857" t="s">
+        <v>5</v>
+      </c>
+      <c r="B857" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C857" t="s">
+        <v>35</v>
+      </c>
+      <c r="D857" t="s">
+        <v>6</v>
+      </c>
+      <c r="E857">
+        <v>1</v>
+      </c>
+      <c r="F857" s="3">
+        <v>2.9525000000000001</v>
+      </c>
+      <c r="G857" s="3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="858" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A858" t="s">
+        <v>5</v>
+      </c>
+      <c r="B858" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C858" t="s">
+        <v>35</v>
+      </c>
+      <c r="D858" t="s">
+        <v>6</v>
+      </c>
+      <c r="E858">
+        <v>1</v>
+      </c>
+      <c r="F858" s="3">
+        <v>2.9348999999999998</v>
+      </c>
+      <c r="G858" s="3">
+        <v>7.6</v>
+      </c>
+    </row>
+    <row r="859" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A859" t="s">
+        <v>5</v>
+      </c>
+      <c r="B859" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C859" t="s">
+        <v>35</v>
+      </c>
+      <c r="D859" t="s">
+        <v>6</v>
+      </c>
+      <c r="E859">
+        <v>1</v>
+      </c>
+      <c r="F859" s="3">
+        <v>2.9190999999999998</v>
+      </c>
+      <c r="G859" s="3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="860" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A860" t="s">
+        <v>5</v>
+      </c>
+      <c r="B860" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C860" t="s">
+        <v>35</v>
+      </c>
+      <c r="D860" t="s">
+        <v>6</v>
+      </c>
+      <c r="E860">
+        <v>1</v>
+      </c>
+      <c r="F860" s="3">
+        <v>2.9051999999999998</v>
+      </c>
+      <c r="G860" s="3">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="861" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A861" t="s">
+        <v>5</v>
+      </c>
+      <c r="B861" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C861" t="s">
+        <v>35</v>
+      </c>
+      <c r="D861" t="s">
+        <v>6</v>
+      </c>
+      <c r="E861">
+        <v>1</v>
+      </c>
+      <c r="F861" s="3">
+        <v>2.8767</v>
+      </c>
+      <c r="G861" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="862" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A862" t="s">
+        <v>5</v>
+      </c>
+      <c r="B862" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C862" t="s">
+        <v>35</v>
+      </c>
+      <c r="D862" t="s">
+        <v>6</v>
+      </c>
+      <c r="E862">
+        <v>1</v>
+      </c>
+      <c r="F862" s="3">
+        <v>2.8380000000000001</v>
+      </c>
+      <c r="G862" s="3">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="863" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A863" t="s">
+        <v>5</v>
+      </c>
+      <c r="B863" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C863" t="s">
+        <v>35</v>
+      </c>
+      <c r="D863" t="s">
+        <v>6</v>
+      </c>
+      <c r="E863">
+        <v>2</v>
+      </c>
+      <c r="F863" s="3">
+        <v>2.1299000000000001</v>
+      </c>
+      <c r="G863" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="864" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A864" t="s">
+        <v>5</v>
+      </c>
+      <c r="B864" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C864" t="s">
+        <v>35</v>
+      </c>
+      <c r="D864" t="s">
+        <v>6</v>
+      </c>
+      <c r="E864">
+        <v>2</v>
+      </c>
+      <c r="F864" s="3">
+        <v>2.1084000000000001</v>
+      </c>
+      <c r="G864" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="865" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A865" t="s">
+        <v>5</v>
+      </c>
+      <c r="B865" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C865" t="s">
+        <v>35</v>
+      </c>
+      <c r="D865" t="s">
+        <v>6</v>
+      </c>
+      <c r="E865">
+        <v>2</v>
+      </c>
+      <c r="F865" s="3">
+        <v>2.0968</v>
+      </c>
+      <c r="G865" s="3">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="866" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A866" t="s">
+        <v>5</v>
+      </c>
+      <c r="B866" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C866" t="s">
+        <v>35</v>
+      </c>
+      <c r="D866" t="s">
+        <v>6</v>
+      </c>
+      <c r="E866">
+        <v>2</v>
+      </c>
+      <c r="F866" s="3">
+        <v>2.0851999999999999</v>
+      </c>
+      <c r="G866" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="867" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A867" t="s">
+        <v>5</v>
+      </c>
+      <c r="B867" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C867" t="s">
+        <v>35</v>
+      </c>
+      <c r="D867" t="s">
+        <v>6</v>
+      </c>
+      <c r="E867">
+        <v>2</v>
+      </c>
+      <c r="F867" s="3">
+        <v>2.0773000000000001</v>
+      </c>
+      <c r="G867" s="3">
+        <v>5.2</v>
+      </c>
+    </row>
+    <row r="868" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A868" t="s">
+        <v>5</v>
+      </c>
+      <c r="B868" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C868" t="s">
+        <v>35</v>
+      </c>
+      <c r="D868" t="s">
+        <v>6</v>
+      </c>
+      <c r="E868">
+        <v>2</v>
+      </c>
+      <c r="F868" s="3">
+        <v>2.0659999999999998</v>
+      </c>
+      <c r="G868" s="3">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="869" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A869" t="s">
+        <v>5</v>
+      </c>
+      <c r="B869" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C869" t="s">
+        <v>35</v>
+      </c>
+      <c r="D869" t="s">
+        <v>6</v>
+      </c>
+      <c r="E869">
+        <v>2</v>
+      </c>
+      <c r="F869" s="3">
+        <v>2.0562999999999998</v>
+      </c>
+      <c r="G869" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="870" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A870" t="s">
+        <v>5</v>
+      </c>
+      <c r="B870" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C870" t="s">
+        <v>35</v>
+      </c>
+      <c r="D870" t="s">
+        <v>6</v>
+      </c>
+      <c r="E870">
+        <v>2</v>
+      </c>
+      <c r="F870" s="3">
+        <v>2.0486</v>
+      </c>
+      <c r="G870" s="3">
+        <v>8.4</v>
+      </c>
+    </row>
+    <row r="871" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A871" t="s">
+        <v>5</v>
+      </c>
+      <c r="B871" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C871" t="s">
+        <v>35</v>
+      </c>
+      <c r="D871" t="s">
+        <v>6</v>
+      </c>
+      <c r="E871">
+        <v>2</v>
+      </c>
+      <c r="F871" s="3">
+        <v>2.0381</v>
+      </c>
+      <c r="G871" s="3">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="872" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A872" t="s">
+        <v>5</v>
+      </c>
+      <c r="B872" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C872" t="s">
+        <v>35</v>
+      </c>
+      <c r="D872" t="s">
+        <v>6</v>
+      </c>
+      <c r="E872">
+        <v>2</v>
+      </c>
+      <c r="F872" s="3">
+        <v>2.0268999999999999</v>
+      </c>
+      <c r="G872" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="873" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A873" t="s">
+        <v>5</v>
+      </c>
+      <c r="B873" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C873" t="s">
+        <v>35</v>
+      </c>
+      <c r="D873" t="s">
+        <v>6</v>
+      </c>
+      <c r="E873">
+        <v>2</v>
+      </c>
+      <c r="F873" s="3">
+        <v>2.0154999999999998</v>
+      </c>
+      <c r="G873" s="3">
+        <v>11.8</v>
+      </c>
+    </row>
+    <row r="874" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A874" t="s">
+        <v>5</v>
+      </c>
+      <c r="B874" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C874" t="s">
+        <v>35</v>
+      </c>
+      <c r="D874" t="s">
+        <v>6</v>
+      </c>
+      <c r="E874">
+        <v>2</v>
+      </c>
+      <c r="F874" s="3">
+        <v>1.9818</v>
+      </c>
+      <c r="G874" s="3">
+        <v>12.6</v>
+      </c>
+    </row>
+    <row r="875" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A875" t="s">
+        <v>5</v>
+      </c>
+      <c r="B875" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C875" t="s">
+        <v>35</v>
+      </c>
+      <c r="D875" t="s">
+        <v>6</v>
+      </c>
+      <c r="E875">
+        <v>2</v>
+      </c>
+      <c r="F875" s="3">
+        <v>1.9530000000000001</v>
+      </c>
+      <c r="G875" s="3">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="876" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A876" t="s">
+        <v>5</v>
+      </c>
+      <c r="B876" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C876" t="s">
+        <v>35</v>
+      </c>
+      <c r="D876" t="s">
+        <v>6</v>
+      </c>
+      <c r="E876">
+        <v>3</v>
+      </c>
+      <c r="F876" s="3">
+        <v>2.4729000000000001</v>
+      </c>
+      <c r="G876" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="877" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A877" t="s">
+        <v>5</v>
+      </c>
+      <c r="B877" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C877" t="s">
+        <v>35</v>
+      </c>
+      <c r="D877" t="s">
+        <v>6</v>
+      </c>
+      <c r="E877">
+        <v>3</v>
+      </c>
+      <c r="F877" s="3">
+        <v>2.4624000000000001</v>
+      </c>
+      <c r="G877" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="878" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A878" t="s">
+        <v>5</v>
+      </c>
+      <c r="B878" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C878" t="s">
+        <v>35</v>
+      </c>
+      <c r="D878" t="s">
+        <v>6</v>
+      </c>
+      <c r="E878">
+        <v>3</v>
+      </c>
+      <c r="F878" s="3">
+        <v>2.4483999999999999</v>
+      </c>
+      <c r="G878" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="879" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A879" t="s">
+        <v>5</v>
+      </c>
+      <c r="B879" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C879" t="s">
+        <v>35</v>
+      </c>
+      <c r="D879" t="s">
+        <v>6</v>
+      </c>
+      <c r="E879">
+        <v>3</v>
+      </c>
+      <c r="F879" s="3">
+        <v>2.4409999999999998</v>
+      </c>
+      <c r="G879" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="880" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A880" t="s">
+        <v>5</v>
+      </c>
+      <c r="B880" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C880" t="s">
+        <v>35</v>
+      </c>
+      <c r="D880" t="s">
+        <v>6</v>
+      </c>
+      <c r="E880">
+        <v>3</v>
+      </c>
+      <c r="F880" s="3">
+        <v>2.4287999999999998</v>
+      </c>
+      <c r="G880" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="881" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A881" t="s">
+        <v>5</v>
+      </c>
+      <c r="B881" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C881" t="s">
+        <v>35</v>
+      </c>
+      <c r="D881" t="s">
+        <v>6</v>
+      </c>
+      <c r="E881">
+        <v>3</v>
+      </c>
+      <c r="F881" s="3">
+        <v>2.4161999999999999</v>
+      </c>
+      <c r="G881" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="882" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A882" t="s">
+        <v>5</v>
+      </c>
+      <c r="B882" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C882" t="s">
+        <v>35</v>
+      </c>
+      <c r="D882" t="s">
+        <v>6</v>
+      </c>
+      <c r="E882">
+        <v>3</v>
+      </c>
+      <c r="F882" s="3">
+        <v>2.4041000000000001</v>
+      </c>
+      <c r="G882" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="883" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A883" t="s">
+        <v>5</v>
+      </c>
+      <c r="B883" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C883" t="s">
+        <v>35</v>
+      </c>
+      <c r="D883" t="s">
+        <v>6</v>
+      </c>
+      <c r="E883">
+        <v>3</v>
+      </c>
+      <c r="F883" s="3">
+        <v>2.3935</v>
+      </c>
+      <c r="G883" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="884" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A884" t="s">
+        <v>5</v>
+      </c>
+      <c r="B884" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C884" t="s">
+        <v>35</v>
+      </c>
+      <c r="D884" t="s">
+        <v>6</v>
+      </c>
+      <c r="E884">
+        <v>3</v>
+      </c>
+      <c r="F884" s="3">
+        <v>2.3654999999999999</v>
+      </c>
+      <c r="G884" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="885" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A885" t="s">
+        <v>5</v>
+      </c>
+      <c r="B885" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C885" t="s">
+        <v>35</v>
+      </c>
+      <c r="D885" t="s">
+        <v>6</v>
+      </c>
+      <c r="E885">
+        <v>3</v>
+      </c>
+      <c r="F885" s="3">
+        <v>2.3567999999999998</v>
+      </c>
+      <c r="G885" s="3">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="886" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A886" t="s">
+        <v>5</v>
+      </c>
+      <c r="B886" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C886" t="s">
+        <v>35</v>
+      </c>
+      <c r="D886" t="s">
+        <v>6</v>
+      </c>
+      <c r="E886">
+        <v>3</v>
+      </c>
+      <c r="F886" s="3">
+        <v>2.3308</v>
+      </c>
+      <c r="G886" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="887" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A887" t="s">
+        <v>5</v>
+      </c>
+      <c r="B887" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C887" t="s">
+        <v>35</v>
+      </c>
+      <c r="D887" t="s">
+        <v>6</v>
+      </c>
+      <c r="E887">
+        <v>3</v>
+      </c>
+      <c r="F887" s="3">
+        <v>2.2746</v>
+      </c>
+      <c r="G887" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="888" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A888" t="s">
+        <v>5</v>
+      </c>
+      <c r="B888" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C888" t="s">
+        <v>35</v>
+      </c>
+      <c r="D888" t="s">
+        <v>6</v>
+      </c>
+      <c r="E888">
+        <v>4</v>
+      </c>
+      <c r="F888" s="3">
+        <v>1.6946000000000001</v>
+      </c>
+      <c r="G888" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="889" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A889" t="s">
+        <v>5</v>
+      </c>
+      <c r="B889" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C889" t="s">
+        <v>35</v>
+      </c>
+      <c r="D889" t="s">
+        <v>6</v>
+      </c>
+      <c r="E889">
+        <v>4</v>
+      </c>
+      <c r="F889" s="3">
+        <v>1.6893</v>
+      </c>
+      <c r="G889" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="890" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A890" t="s">
+        <v>5</v>
+      </c>
+      <c r="B890" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C890" t="s">
+        <v>35</v>
+      </c>
+      <c r="D890" t="s">
+        <v>6</v>
+      </c>
+      <c r="E890">
+        <v>4</v>
+      </c>
+      <c r="F890" s="3">
+        <v>1.6838</v>
+      </c>
+      <c r="G890" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="891" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A891" t="s">
+        <v>5</v>
+      </c>
+      <c r="B891" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C891" t="s">
+        <v>35</v>
+      </c>
+      <c r="D891" t="s">
+        <v>6</v>
+      </c>
+      <c r="E891">
+        <v>4</v>
+      </c>
+      <c r="F891" s="3">
+        <v>1.6771</v>
+      </c>
+      <c r="G891" s="3">
+        <v>8.1999999999999993</v>
+      </c>
+    </row>
+    <row r="892" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A892" t="s">
+        <v>5</v>
+      </c>
+      <c r="B892" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C892" t="s">
+        <v>35</v>
+      </c>
+      <c r="D892" t="s">
+        <v>6</v>
+      </c>
+      <c r="E892">
+        <v>4</v>
+      </c>
+      <c r="F892" s="3">
+        <v>1.6721999999999999</v>
+      </c>
+      <c r="G892" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="893" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A893" t="s">
+        <v>5</v>
+      </c>
+      <c r="B893" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C893" t="s">
+        <v>35</v>
+      </c>
+      <c r="D893" t="s">
+        <v>6</v>
+      </c>
+      <c r="E893">
+        <v>4</v>
+      </c>
+      <c r="F893" s="3">
+        <v>1.6698</v>
+      </c>
+      <c r="G893" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="894" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A894" t="s">
+        <v>5</v>
+      </c>
+      <c r="B894" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C894" t="s">
+        <v>35</v>
+      </c>
+      <c r="D894" t="s">
+        <v>6</v>
+      </c>
+      <c r="E894">
+        <v>4</v>
+      </c>
+      <c r="F894" s="3">
+        <v>1.6433</v>
+      </c>
+      <c r="G894" s="3">
+        <v>12.9</v>
+      </c>
+    </row>
+    <row r="895" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A895" t="s">
+        <v>5</v>
+      </c>
+      <c r="B895" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C895" t="s">
+        <v>35</v>
+      </c>
+      <c r="D895" t="s">
+        <v>6</v>
+      </c>
+      <c r="E895">
+        <v>4</v>
+      </c>
+      <c r="F895" s="3">
+        <v>1.6294999999999999</v>
+      </c>
+      <c r="G895" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="896" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A896" t="s">
+        <v>5</v>
+      </c>
+      <c r="B896" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C896" t="s">
+        <v>35</v>
+      </c>
+      <c r="D896" t="s">
+        <v>6</v>
+      </c>
+      <c r="E896">
+        <v>4</v>
+      </c>
+      <c r="F896" s="3">
+        <v>1.5940000000000001</v>
+      </c>
+      <c r="G896" s="3">
+        <v>15.9</v>
+      </c>
+    </row>
+    <row r="897" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A897" t="s">
+        <v>5</v>
+      </c>
+      <c r="B897" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C897" t="s">
+        <v>35</v>
+      </c>
+      <c r="D897" t="s">
+        <v>6</v>
+      </c>
+      <c r="E897">
+        <v>5</v>
+      </c>
+      <c r="F897" s="3">
+        <v>2.3755000000000002</v>
+      </c>
+      <c r="G897" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="898" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A898" t="s">
+        <v>5</v>
+      </c>
+      <c r="B898" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C898" t="s">
+        <v>35</v>
+      </c>
+      <c r="D898" t="s">
+        <v>6</v>
+      </c>
+      <c r="E898">
+        <v>5</v>
+      </c>
+      <c r="F898" s="3">
+        <v>2.3622000000000001</v>
+      </c>
+      <c r="G898" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="899" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A899" t="s">
+        <v>5</v>
+      </c>
+      <c r="B899" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C899" t="s">
+        <v>35</v>
+      </c>
+      <c r="D899" t="s">
+        <v>6</v>
+      </c>
+      <c r="E899">
+        <v>5</v>
+      </c>
+      <c r="F899" s="3">
+        <v>2.3512</v>
+      </c>
+      <c r="G899" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="900" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A900" t="s">
+        <v>5</v>
+      </c>
+      <c r="B900" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C900" t="s">
+        <v>35</v>
+      </c>
+      <c r="D900" t="s">
+        <v>6</v>
+      </c>
+      <c r="E900">
+        <v>5</v>
+      </c>
+      <c r="F900" s="3">
+        <v>2.3412000000000002</v>
+      </c>
+      <c r="G900" s="3">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="901" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A901" t="s">
+        <v>5</v>
+      </c>
+      <c r="B901" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C901" t="s">
+        <v>35</v>
+      </c>
+      <c r="D901" t="s">
+        <v>6</v>
+      </c>
+      <c r="E901">
+        <v>5</v>
+      </c>
+      <c r="F901" s="3">
+        <v>2.3357999999999999</v>
+      </c>
+      <c r="G901" s="3">
+        <v>7.8</v>
+      </c>
+    </row>
+    <row r="902" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A902" t="s">
+        <v>5</v>
+      </c>
+      <c r="B902" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C902" t="s">
+        <v>35</v>
+      </c>
+      <c r="D902" t="s">
+        <v>6</v>
+      </c>
+      <c r="E902">
+        <v>5</v>
+      </c>
+      <c r="F902" s="3">
+        <v>2.3254999999999999</v>
+      </c>
+      <c r="G902" s="3">
+        <v>8.3000000000000007</v>
+      </c>
+    </row>
+    <row r="903" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A903" t="s">
+        <v>5</v>
+      </c>
+      <c r="B903" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C903" t="s">
+        <v>35</v>
+      </c>
+      <c r="D903" t="s">
+        <v>6</v>
+      </c>
+      <c r="E903">
+        <v>5</v>
+      </c>
+      <c r="F903" s="3">
+        <v>2.319</v>
+      </c>
+      <c r="G903" s="3">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="904" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A904" t="s">
+        <v>5</v>
+      </c>
+      <c r="B904" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C904" t="s">
+        <v>35</v>
+      </c>
+      <c r="D904" t="s">
+        <v>6</v>
+      </c>
+      <c r="E904">
+        <v>5</v>
+      </c>
+      <c r="F904" s="3">
+        <v>2.3046000000000002</v>
+      </c>
+      <c r="G904" s="3">
+        <v>10.8</v>
+      </c>
+    </row>
+    <row r="905" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A905" t="s">
+        <v>5</v>
+      </c>
+      <c r="B905" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C905" t="s">
+        <v>35</v>
+      </c>
+      <c r="D905" t="s">
+        <v>6</v>
+      </c>
+      <c r="E905">
+        <v>5</v>
+      </c>
+      <c r="F905" s="3">
+        <v>2.2866</v>
+      </c>
+      <c r="G905" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="906" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A906" t="s">
+        <v>5</v>
+      </c>
+      <c r="B906" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C906" t="s">
+        <v>35</v>
+      </c>
+      <c r="D906" t="s">
+        <v>6</v>
+      </c>
+      <c r="E906">
+        <v>6</v>
+      </c>
+      <c r="F906" s="3">
+        <v>3.9649000000000001</v>
+      </c>
+      <c r="G906" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="907" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A907" t="s">
+        <v>5</v>
+      </c>
+      <c r="B907" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C907" t="s">
+        <v>35</v>
+      </c>
+      <c r="D907" t="s">
+        <v>6</v>
+      </c>
+      <c r="E907">
+        <v>6</v>
+      </c>
+      <c r="F907" s="3">
+        <v>3.9367000000000001</v>
+      </c>
+      <c r="G907" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="908" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A908" t="s">
+        <v>5</v>
+      </c>
+      <c r="B908" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C908" t="s">
+        <v>35</v>
+      </c>
+      <c r="D908" t="s">
+        <v>6</v>
+      </c>
+      <c r="E908">
+        <v>6</v>
+      </c>
+      <c r="F908" s="3">
+        <v>3.9251999999999998</v>
+      </c>
+      <c r="G908" s="3">
+        <v>2.8</v>
+      </c>
+    </row>
+    <row r="909" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A909" t="s">
+        <v>5</v>
+      </c>
+      <c r="B909" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C909" t="s">
+        <v>35</v>
+      </c>
+      <c r="D909" t="s">
+        <v>6</v>
+      </c>
+      <c r="E909">
+        <v>6</v>
+      </c>
+      <c r="F909" s="3">
+        <v>3.9062999999999999</v>
+      </c>
+      <c r="G909" s="3">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="910" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A910" t="s">
+        <v>5</v>
+      </c>
+      <c r="B910" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C910" t="s">
+        <v>35</v>
+      </c>
+      <c r="D910" t="s">
+        <v>6</v>
+      </c>
+      <c r="E910">
+        <v>6</v>
+      </c>
+      <c r="F910" s="3">
+        <v>3.8855</v>
+      </c>
+      <c r="G910" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="911" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A911" t="s">
+        <v>5</v>
+      </c>
+      <c r="B911" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C911" t="s">
+        <v>35</v>
+      </c>
+      <c r="D911" t="s">
+        <v>6</v>
+      </c>
+      <c r="E911">
+        <v>6</v>
+      </c>
+      <c r="F911" s="3">
+        <v>3.8668</v>
+      </c>
+      <c r="G911" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="912" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A912" t="s">
+        <v>5</v>
+      </c>
+      <c r="B912" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C912" t="s">
+        <v>35</v>
+      </c>
+      <c r="D912" t="s">
+        <v>6</v>
+      </c>
+      <c r="E912">
+        <v>6</v>
+      </c>
+      <c r="F912" s="3">
+        <v>3.8502999999999998</v>
+      </c>
+      <c r="G912" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="913" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A913" t="s">
+        <v>5</v>
+      </c>
+      <c r="B913" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C913" t="s">
+        <v>35</v>
+      </c>
+      <c r="D913" t="s">
+        <v>6</v>
+      </c>
+      <c r="E913">
+        <v>6</v>
+      </c>
+      <c r="F913" s="3">
+        <v>3.8338999999999999</v>
+      </c>
+      <c r="G913" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="914" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A914" t="s">
+        <v>5</v>
+      </c>
+      <c r="B914" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C914" t="s">
+        <v>35</v>
+      </c>
+      <c r="D914" t="s">
+        <v>6</v>
+      </c>
+      <c r="E914">
+        <v>6</v>
+      </c>
+      <c r="F914" s="3">
+        <v>3.8180999999999998</v>
+      </c>
+      <c r="G914" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="915" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A915" t="s">
+        <v>5</v>
+      </c>
+      <c r="B915" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C915" t="s">
+        <v>35</v>
+      </c>
+      <c r="D915" t="s">
+        <v>6</v>
+      </c>
+      <c r="E915">
+        <v>6</v>
+      </c>
+      <c r="F915" s="3">
+        <v>3.7991999999999999</v>
+      </c>
+      <c r="G915" s="3">
+        <v>8.8000000000000007</v>
+      </c>
+    </row>
+    <row r="916" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A916" t="s">
+        <v>5</v>
+      </c>
+      <c r="B916" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C916" t="s">
+        <v>35</v>
+      </c>
+      <c r="D916" t="s">
+        <v>6</v>
+      </c>
+      <c r="E916">
+        <v>6</v>
+      </c>
+      <c r="F916" s="3">
+        <v>3.7454000000000001</v>
+      </c>
+      <c r="G916" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="917" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A917" t="s">
+        <v>5</v>
+      </c>
+      <c r="B917" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C917" t="s">
+        <v>35</v>
+      </c>
+      <c r="D917" t="s">
+        <v>6</v>
+      </c>
+      <c r="E917">
+        <v>6</v>
+      </c>
+      <c r="F917" s="3">
+        <v>3.7122000000000002</v>
+      </c>
+      <c r="G917" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="918" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A918" t="s">
+        <v>5</v>
+      </c>
+      <c r="B918" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C918" t="s">
+        <v>35</v>
+      </c>
+      <c r="D918" t="s">
+        <v>6</v>
+      </c>
+      <c r="E918">
+        <v>6</v>
+      </c>
+      <c r="F918" s="3">
+        <v>3.633</v>
+      </c>
+      <c r="G918" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="919" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A919" t="s">
+        <v>5</v>
+      </c>
+      <c r="B919" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C919" t="s">
+        <v>37</v>
+      </c>
+      <c r="D919" t="s">
+        <v>11</v>
+      </c>
+      <c r="E919">
+        <v>1</v>
+      </c>
+      <c r="F919" s="3">
+        <v>0.82689999999999997</v>
+      </c>
+      <c r="G919" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="920" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A920" t="s">
+        <v>5</v>
+      </c>
+      <c r="B920" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C920" t="s">
+        <v>37</v>
+      </c>
+      <c r="D920" t="s">
+        <v>11</v>
+      </c>
+      <c r="E920">
+        <v>1</v>
+      </c>
+      <c r="F920" s="3">
+        <v>0.81220000000000003</v>
+      </c>
+      <c r="G920" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="921" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A921" t="s">
+        <v>5</v>
+      </c>
+      <c r="B921" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C921" t="s">
+        <v>37</v>
+      </c>
+      <c r="D921" t="s">
+        <v>11</v>
+      </c>
+      <c r="E921">
+        <v>1</v>
+      </c>
+      <c r="F921" s="3">
+        <v>0.80279999999999996</v>
+      </c>
+      <c r="G921" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="922" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A922" t="s">
+        <v>5</v>
+      </c>
+      <c r="B922" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C922" t="s">
+        <v>37</v>
+      </c>
+      <c r="D922" t="s">
+        <v>11</v>
+      </c>
+      <c r="E922">
+        <v>1</v>
+      </c>
+      <c r="F922" s="3">
+        <v>0.78990000000000005</v>
+      </c>
+      <c r="G922" s="3">
+        <v>14.5</v>
+      </c>
+    </row>
+    <row r="923" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A923" t="s">
+        <v>5</v>
+      </c>
+      <c r="B923" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C923" t="s">
+        <v>37</v>
+      </c>
+      <c r="D923" t="s">
+        <v>11</v>
+      </c>
+      <c r="E923">
+        <v>1</v>
+      </c>
+      <c r="F923" s="3">
+        <v>0.7752</v>
+      </c>
+      <c r="G923" s="3">
+        <v>15.2</v>
+      </c>
+    </row>
+    <row r="924" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A924" t="s">
+        <v>5</v>
+      </c>
+      <c r="B924" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C924" t="s">
+        <v>37</v>
+      </c>
+      <c r="D924" t="s">
+        <v>11</v>
+      </c>
+      <c r="E924">
+        <v>1</v>
+      </c>
+      <c r="F924" s="3">
+        <v>0.75290000000000001</v>
+      </c>
+      <c r="G924" s="3">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="925" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A925" t="s">
+        <v>5</v>
+      </c>
+      <c r="B925" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C925" t="s">
+        <v>37</v>
+      </c>
+      <c r="D925" t="s">
+        <v>11</v>
+      </c>
+      <c r="E925">
+        <v>1</v>
+      </c>
+      <c r="F925" s="3">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="G925" s="3">
+        <v>17.7</v>
+      </c>
+    </row>
+    <row r="926" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A926" t="s">
+        <v>5</v>
+      </c>
+      <c r="B926" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C926" t="s">
+        <v>37</v>
+      </c>
+      <c r="D926" t="s">
+        <v>11</v>
+      </c>
+      <c r="E926">
+        <v>1</v>
+      </c>
+      <c r="F926" s="3">
+        <v>0.66410000000000002</v>
+      </c>
+      <c r="G926" s="3">
+        <v>19.899999999999999</v>
+      </c>
+    </row>
+    <row r="927" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A927" t="s">
+        <v>5</v>
+      </c>
+      <c r="B927" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C927" t="s">
+        <v>37</v>
+      </c>
+      <c r="D927" t="s">
+        <v>11</v>
+      </c>
+      <c r="E927">
+        <v>2</v>
+      </c>
+      <c r="F927" s="3">
+        <v>2.4089</v>
+      </c>
+      <c r="G927" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="928" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A928" t="s">
+        <v>5</v>
+      </c>
+      <c r="B928" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C928" t="s">
+        <v>37</v>
+      </c>
+      <c r="D928" t="s">
+        <v>11</v>
+      </c>
+      <c r="E928">
+        <v>2</v>
+      </c>
+      <c r="F928" s="3">
+        <v>2.36</v>
+      </c>
+      <c r="G928" s="3">
+        <v>5.0999999999999996</v>
+      </c>
+    </row>
+    <row r="929" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A929" t="s">
+        <v>5</v>
+      </c>
+      <c r="B929" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C929" t="s">
+        <v>37</v>
+      </c>
+      <c r="D929" t="s">
+        <v>11</v>
+      </c>
+      <c r="E929">
+        <v>2</v>
+      </c>
+      <c r="F929" s="3">
+        <v>2.3130999999999999</v>
+      </c>
+      <c r="G929" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="930" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A930" t="s">
+        <v>5</v>
+      </c>
+      <c r="B930" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C930" t="s">
+        <v>37</v>
+      </c>
+      <c r="D930" t="s">
+        <v>11</v>
+      </c>
+      <c r="E930">
+        <v>2</v>
+      </c>
+      <c r="F930" s="3">
+        <v>2.2787000000000002</v>
+      </c>
+      <c r="G930" s="3">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="931" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A931" t="s">
+        <v>5</v>
+      </c>
+      <c r="B931" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C931" t="s">
+        <v>37</v>
+      </c>
+      <c r="D931" t="s">
+        <v>11</v>
+      </c>
+      <c r="E931">
+        <v>2</v>
+      </c>
+      <c r="F931" s="3">
+        <v>2.2418999999999998</v>
+      </c>
+      <c r="G931" s="3">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="932" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A932" t="s">
+        <v>5</v>
+      </c>
+      <c r="B932" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C932" t="s">
+        <v>37</v>
+      </c>
+      <c r="D932" t="s">
+        <v>11</v>
+      </c>
+      <c r="E932">
+        <v>2</v>
+      </c>
+      <c r="F932" s="3">
+        <v>2.1966999999999999</v>
+      </c>
+      <c r="G932" s="3">
+        <v>14.2</v>
+      </c>
+    </row>
+    <row r="933" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A933" t="s">
+        <v>5</v>
+      </c>
+      <c r="B933" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C933" t="s">
+        <v>37</v>
+      </c>
+      <c r="D933" t="s">
+        <v>11</v>
+      </c>
+      <c r="E933">
+        <v>2</v>
+      </c>
+      <c r="F933" s="3">
+        <v>2.1353</v>
+      </c>
+      <c r="G933" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="934" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A934" t="s">
+        <v>5</v>
+      </c>
+      <c r="B934" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C934" t="s">
+        <v>37</v>
+      </c>
+      <c r="D934" t="s">
+        <v>11</v>
+      </c>
+      <c r="E934">
+        <v>2</v>
+      </c>
+      <c r="F934" s="3">
+        <v>2.0889000000000002</v>
+      </c>
+      <c r="G934" s="3">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="935" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A935" t="s">
+        <v>5</v>
+      </c>
+      <c r="B935" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C935" t="s">
+        <v>37</v>
+      </c>
+      <c r="D935" t="s">
+        <v>11</v>
+      </c>
+      <c r="E935">
+        <v>2</v>
+      </c>
+      <c r="F935" s="3">
+        <v>1.9901</v>
+      </c>
+      <c r="G935" s="3">
+        <v>16.600000000000001</v>
+      </c>
+    </row>
+    <row r="936" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A936" t="s">
+        <v>5</v>
+      </c>
+      <c r="B936" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C936" t="s">
+        <v>37</v>
+      </c>
+      <c r="D936" t="s">
+        <v>11</v>
+      </c>
+      <c r="E936">
+        <v>2</v>
+      </c>
+      <c r="F936" s="3">
+        <v>1.6732</v>
+      </c>
+      <c r="G936" s="3">
+        <v>21.8</v>
+      </c>
+    </row>
+    <row r="937" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A937" t="s">
+        <v>5</v>
+      </c>
+      <c r="B937" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C937" t="s">
+        <v>37</v>
+      </c>
+      <c r="D937" t="s">
+        <v>11</v>
+      </c>
+      <c r="E937">
+        <v>3</v>
+      </c>
+      <c r="F937" s="3">
+        <v>1.9231</v>
+      </c>
+      <c r="G937" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="938" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A938" t="s">
+        <v>5</v>
+      </c>
+      <c r="B938" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C938" t="s">
+        <v>37</v>
+      </c>
+      <c r="D938" t="s">
+        <v>11</v>
+      </c>
+      <c r="E938">
+        <v>3</v>
+      </c>
+      <c r="F938" s="3">
+        <v>1.8673999999999999</v>
+      </c>
+      <c r="G938" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="939" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A939" t="s">
+        <v>5</v>
+      </c>
+      <c r="B939" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C939" t="s">
+        <v>37</v>
+      </c>
+      <c r="D939" t="s">
+        <v>11</v>
+      </c>
+      <c r="E939">
+        <v>3</v>
+      </c>
+      <c r="F939" s="3">
+        <v>1.8383</v>
+      </c>
+      <c r="G939" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="940" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A940" t="s">
+        <v>5</v>
+      </c>
+      <c r="B940" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C940" t="s">
+        <v>37</v>
+      </c>
+      <c r="D940" t="s">
+        <v>11</v>
+      </c>
+      <c r="E940">
+        <v>3</v>
+      </c>
+      <c r="F940" s="3">
+        <v>1.7787999999999999</v>
+      </c>
+      <c r="G940" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="941" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A941" t="s">
+        <v>5</v>
+      </c>
+      <c r="B941" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C941" t="s">
+        <v>37</v>
+      </c>
+      <c r="D941" t="s">
+        <v>11</v>
+      </c>
+      <c r="E941">
+        <v>3</v>
+      </c>
+      <c r="F941" s="3">
+        <v>1.7668999999999999</v>
+      </c>
+      <c r="G941" s="3">
+        <v>15.8</v>
+      </c>
+    </row>
+    <row r="942" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A942" t="s">
+        <v>5</v>
+      </c>
+      <c r="B942" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C942" t="s">
+        <v>37</v>
+      </c>
+      <c r="D942" t="s">
+        <v>11</v>
+      </c>
+      <c r="E942">
+        <v>3</v>
+      </c>
+      <c r="F942" s="3">
+        <v>1.7009000000000001</v>
+      </c>
+      <c r="G942" s="3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="943" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A943" t="s">
+        <v>5</v>
+      </c>
+      <c r="B943" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C943" t="s">
+        <v>37</v>
+      </c>
+      <c r="D943" t="s">
+        <v>11</v>
+      </c>
+      <c r="E943">
+        <v>3</v>
+      </c>
+      <c r="F943" s="3">
+        <v>1.6409</v>
+      </c>
+      <c r="G943" s="3">
+        <v>17.100000000000001</v>
+      </c>
+    </row>
+    <row r="944" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A944" t="s">
+        <v>5</v>
+      </c>
+      <c r="B944" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C944" t="s">
+        <v>37</v>
+      </c>
+      <c r="D944" t="s">
+        <v>11</v>
+      </c>
+      <c r="E944">
+        <v>3</v>
+      </c>
+      <c r="F944" s="3">
+        <v>1.4319</v>
+      </c>
+      <c r="G944" s="3">
+        <v>21.5</v>
+      </c>
+    </row>
+    <row r="945" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A945" t="s">
+        <v>5</v>
+      </c>
+      <c r="B945" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C945" t="s">
+        <v>37</v>
+      </c>
+      <c r="D945" t="s">
+        <v>11</v>
+      </c>
+      <c r="E945">
+        <v>5</v>
+      </c>
+      <c r="F945" s="3">
+        <v>1.0029999999999999</v>
+      </c>
+      <c r="G945" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="946" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A946" t="s">
+        <v>5</v>
+      </c>
+      <c r="B946" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C946" t="s">
+        <v>37</v>
+      </c>
+      <c r="D946" t="s">
+        <v>11</v>
+      </c>
+      <c r="E946">
+        <v>5</v>
+      </c>
+      <c r="F946" s="3">
+        <v>0.97599999999999998</v>
+      </c>
+      <c r="G946" s="3">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="947" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A947" t="s">
+        <v>5</v>
+      </c>
+      <c r="B947" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C947" t="s">
+        <v>37</v>
+      </c>
+      <c r="D947" t="s">
+        <v>11</v>
+      </c>
+      <c r="E947">
+        <v>5</v>
+      </c>
+      <c r="F947" s="3">
+        <v>0.96540000000000004</v>
+      </c>
+      <c r="G947" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="948" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A948" t="s">
+        <v>5</v>
+      </c>
+      <c r="B948" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C948" t="s">
+        <v>37</v>
+      </c>
+      <c r="D948" t="s">
+        <v>11</v>
+      </c>
+      <c r="E948">
+        <v>5</v>
+      </c>
+      <c r="F948" s="3">
+        <v>0.9546</v>
+      </c>
+      <c r="G948" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="949" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A949" t="s">
+        <v>5</v>
+      </c>
+      <c r="B949" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C949" t="s">
+        <v>37</v>
+      </c>
+      <c r="D949" t="s">
+        <v>11</v>
+      </c>
+      <c r="E949">
+        <v>5</v>
+      </c>
+      <c r="F949" s="3">
+        <v>0.94420000000000004</v>
+      </c>
+      <c r="G949" s="3">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="950" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A950" t="s">
+        <v>5</v>
+      </c>
+      <c r="B950" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C950" t="s">
+        <v>37</v>
+      </c>
+      <c r="D950" t="s">
+        <v>11</v>
+      </c>
+      <c r="E950">
+        <v>5</v>
+      </c>
+      <c r="F950" s="3">
+        <v>0.93140000000000001</v>
+      </c>
+      <c r="G950" s="3">
+        <v>16.399999999999999</v>
+      </c>
+    </row>
+    <row r="951" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A951" t="s">
+        <v>5</v>
+      </c>
+      <c r="B951" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C951" t="s">
+        <v>37</v>
+      </c>
+      <c r="D951" t="s">
+        <v>11</v>
+      </c>
+      <c r="E951">
+        <v>5</v>
+      </c>
+      <c r="F951" s="3">
+        <v>0.89849999999999997</v>
+      </c>
+      <c r="G951" s="3">
+        <v>17.2</v>
+      </c>
+    </row>
+    <row r="952" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A952" t="s">
+        <v>5</v>
+      </c>
+      <c r="B952" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C952" t="s">
+        <v>37</v>
+      </c>
+      <c r="D952" t="s">
+        <v>11</v>
+      </c>
+      <c r="E952">
+        <v>5</v>
+      </c>
+      <c r="F952" s="3">
+        <v>0.8448</v>
+      </c>
+      <c r="G952" s="3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="953" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A953" t="s">
+        <v>5</v>
+      </c>
+      <c r="B953" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C953" t="s">
+        <v>37</v>
+      </c>
+      <c r="D953" t="s">
+        <v>11</v>
+      </c>
+      <c r="E953">
+        <v>6</v>
+      </c>
+      <c r="F953" s="3">
+        <v>1.7655000000000001</v>
+      </c>
+      <c r="G953" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="954" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A954" t="s">
+        <v>5</v>
+      </c>
+      <c r="B954" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C954" t="s">
+        <v>37</v>
+      </c>
+      <c r="D954" t="s">
+        <v>11</v>
+      </c>
+      <c r="E954">
+        <v>6</v>
+      </c>
+      <c r="F954" s="3">
+        <v>1.7212000000000001</v>
+      </c>
+      <c r="G954" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="955" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A955" t="s">
+        <v>5</v>
+      </c>
+      <c r="B955" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C955" t="s">
+        <v>37</v>
+      </c>
+      <c r="D955" t="s">
+        <v>11</v>
+      </c>
+      <c r="E955">
+        <v>6</v>
+      </c>
+      <c r="F955" s="3">
+        <v>1.6972</v>
+      </c>
+      <c r="G955" s="3">
+        <v>9.9</v>
+      </c>
+    </row>
+    <row r="956" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A956" t="s">
+        <v>5</v>
+      </c>
+      <c r="B956" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C956" t="s">
+        <v>37</v>
+      </c>
+      <c r="D956" t="s">
+        <v>11</v>
+      </c>
+      <c r="E956">
+        <v>6</v>
+      </c>
+      <c r="F956" s="3">
+        <v>1.6868000000000001</v>
+      </c>
+      <c r="G956" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="957" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A957" t="s">
+        <v>5</v>
+      </c>
+      <c r="B957" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C957" t="s">
+        <v>37</v>
+      </c>
+      <c r="D957" t="s">
+        <v>11</v>
+      </c>
+      <c r="E957">
+        <v>6</v>
+      </c>
+      <c r="F957" s="3">
+        <v>1.6667000000000001</v>
+      </c>
+      <c r="G957" s="3">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="958" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A958" t="s">
+        <v>5</v>
+      </c>
+      <c r="B958" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C958" t="s">
+        <v>37</v>
+      </c>
+      <c r="D958" t="s">
+        <v>11</v>
+      </c>
+      <c r="E958">
+        <v>6</v>
+      </c>
+      <c r="F958" s="3">
+        <v>1.6365000000000001</v>
+      </c>
+      <c r="G958" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="959" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A959" t="s">
+        <v>5</v>
+      </c>
+      <c r="B959" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C959" t="s">
+        <v>37</v>
+      </c>
+      <c r="D959" t="s">
+        <v>11</v>
+      </c>
+      <c r="E959">
+        <v>6</v>
+      </c>
+      <c r="F959" s="3">
+        <v>1.6092</v>
+      </c>
+      <c r="G959" s="3">
+        <v>12.3</v>
+      </c>
+    </row>
+    <row r="960" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A960" t="s">
+        <v>5</v>
+      </c>
+      <c r="B960" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C960" t="s">
+        <v>37</v>
+      </c>
+      <c r="D960" t="s">
+        <v>11</v>
+      </c>
+      <c r="E960">
+        <v>6</v>
+      </c>
+      <c r="F960" s="3">
+        <v>1.5758000000000001</v>
+      </c>
+      <c r="G960" s="3">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="961" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A961" t="s">
+        <v>5</v>
+      </c>
+      <c r="B961" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C961" t="s">
+        <v>37</v>
+      </c>
+      <c r="D961" t="s">
+        <v>11</v>
+      </c>
+      <c r="E961">
+        <v>6</v>
+      </c>
+      <c r="F961" s="3">
+        <v>1.5431999999999999</v>
+      </c>
+      <c r="G961" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="962" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A962" t="s">
+        <v>5</v>
+      </c>
+      <c r="B962" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C962" t="s">
+        <v>37</v>
+      </c>
+      <c r="D962" t="s">
+        <v>11</v>
+      </c>
+      <c r="E962">
+        <v>6</v>
+      </c>
+      <c r="F962" s="3">
+        <v>1.5047999999999999</v>
+      </c>
+      <c r="G962" s="3">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="963" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A963" t="s">
+        <v>5</v>
+      </c>
+      <c r="B963" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C963" t="s">
+        <v>37</v>
+      </c>
+      <c r="D963" t="s">
+        <v>11</v>
+      </c>
+      <c r="E963">
+        <v>6</v>
+      </c>
+      <c r="F963" s="3">
+        <v>1.4608000000000001</v>
+      </c>
+      <c r="G963" s="3">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="964" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A964" t="s">
+        <v>5</v>
+      </c>
+      <c r="B964" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C964" t="s">
+        <v>37</v>
+      </c>
+      <c r="D964" t="s">
+        <v>11</v>
+      </c>
+      <c r="E964">
+        <v>6</v>
+      </c>
+      <c r="F964" s="3">
+        <v>1.3933</v>
+      </c>
+      <c r="G964" s="3">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="965" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A965" t="s">
+        <v>5</v>
+      </c>
+      <c r="B965" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C965" t="s">
+        <v>37</v>
+      </c>
+      <c r="D965" t="s">
+        <v>11</v>
+      </c>
+      <c r="E965">
+        <v>6</v>
+      </c>
+      <c r="F965" s="3">
+        <v>1.3363</v>
+      </c>
+      <c r="G965" s="3">
+        <v>16.2</v>
+      </c>
+    </row>
+    <row r="966" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A966" t="s">
+        <v>5</v>
+      </c>
+      <c r="B966" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C966" t="s">
+        <v>37</v>
+      </c>
+      <c r="D966" t="s">
+        <v>11</v>
+      </c>
+      <c r="E966">
+        <v>8</v>
+      </c>
+      <c r="G966" s="3"/>
+    </row>
+    <row r="967" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A967" t="s">
+        <v>5</v>
+      </c>
+      <c r="B967" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C967" t="s">
+        <v>37</v>
+      </c>
+      <c r="D967" t="s">
+        <v>11</v>
+      </c>
+      <c r="E967">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="968" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A968" t="s">
+        <v>5</v>
+      </c>
+      <c r="B968" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C968" t="s">
+        <v>37</v>
+      </c>
+      <c r="D968" t="s">
+        <v>11</v>
+      </c>
+      <c r="E968">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="969" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A969" t="s">
+        <v>5</v>
+      </c>
+      <c r="B969" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C969" t="s">
+        <v>37</v>
+      </c>
+      <c r="D969" t="s">
+        <v>11</v>
+      </c>
+      <c r="E969">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="970" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A970" t="s">
+        <v>5</v>
+      </c>
+      <c r="B970" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C970" t="s">
+        <v>37</v>
+      </c>
+      <c r="D970" t="s">
+        <v>11</v>
+      </c>
+      <c r="E970">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="971" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A971" t="s">
+        <v>5</v>
+      </c>
+      <c r="B971" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C971" t="s">
+        <v>37</v>
+      </c>
+      <c r="D971" t="s">
+        <v>11</v>
+      </c>
+      <c r="E971">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="972" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A972" t="s">
+        <v>5</v>
+      </c>
+      <c r="B972" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C972" t="s">
+        <v>37</v>
+      </c>
+      <c r="D972" t="s">
+        <v>11</v>
+      </c>
+      <c r="E972">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="973" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A973" t="s">
+        <v>5</v>
+      </c>
+      <c r="B973" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C973" t="s">
+        <v>37</v>
+      </c>
+      <c r="D973" t="s">
+        <v>11</v>
+      </c>
+      <c r="E973">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="974" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A974" t="s">
+        <v>5</v>
+      </c>
+      <c r="B974" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C974" t="s">
+        <v>37</v>
+      </c>
+      <c r="D974" t="s">
+        <v>11</v>
+      </c>
+      <c r="E974">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="975" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A975" t="s">
+        <v>5</v>
+      </c>
+      <c r="B975" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C975" t="s">
+        <v>37</v>
+      </c>
+      <c r="D975" t="s">
+        <v>11</v>
+      </c>
+      <c r="E975">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="976" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A976" t="s">
+        <v>5</v>
+      </c>
+      <c r="B976" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C976" t="s">
+        <v>37</v>
+      </c>
+      <c r="D976" t="s">
+        <v>11</v>
+      </c>
+      <c r="E976">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="977" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A977" t="s">
+        <v>5</v>
+      </c>
+      <c r="B977" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C977" t="s">
+        <v>37</v>
+      </c>
+      <c r="D977" t="s">
+        <v>11</v>
+      </c>
+      <c r="E977">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="978" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A978" t="s">
+        <v>5</v>
+      </c>
+      <c r="B978" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C978" t="s">
+        <v>37</v>
+      </c>
+      <c r="D978" t="s">
+        <v>11</v>
+      </c>
+      <c r="E978">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="979" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A979" t="s">
+        <v>5</v>
+      </c>
+      <c r="B979" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C979" t="s">
+        <v>37</v>
+      </c>
+      <c r="D979" t="s">
+        <v>11</v>
+      </c>
+      <c r="E979">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="980" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A980" t="s">
+        <v>5</v>
+      </c>
+      <c r="B980" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C980" t="s">
+        <v>37</v>
+      </c>
+      <c r="D980" t="s">
+        <v>11</v>
+      </c>
+      <c r="E980">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="981" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A981" t="s">
+        <v>5</v>
+      </c>
+      <c r="B981" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C981" t="s">
+        <v>37</v>
+      </c>
+      <c r="D981" t="s">
+        <v>11</v>
+      </c>
+      <c r="E981">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="982" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A982" t="s">
+        <v>5</v>
+      </c>
+      <c r="B982" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C982" t="s">
+        <v>37</v>
+      </c>
+      <c r="D982" t="s">
+        <v>11</v>
+      </c>
+      <c r="E982">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="983" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A983" t="s">
+        <v>5</v>
+      </c>
+      <c r="B983" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C983" t="s">
+        <v>37</v>
+      </c>
+      <c r="D983" t="s">
+        <v>11</v>
+      </c>
+      <c r="E983">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="984" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A984" t="s">
+        <v>5</v>
+      </c>
+      <c r="B984" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C984" t="s">
+        <v>37</v>
+      </c>
+      <c r="D984" t="s">
+        <v>11</v>
+      </c>
+      <c r="E984">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="985" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A985" t="s">
+        <v>5</v>
+      </c>
+      <c r="B985" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C985" t="s">
+        <v>37</v>
+      </c>
+      <c r="D985" t="s">
+        <v>11</v>
+      </c>
+      <c r="E985">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="986" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A986" t="s">
+        <v>5</v>
+      </c>
+      <c r="B986" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C986" t="s">
+        <v>37</v>
+      </c>
+      <c r="D986" t="s">
+        <v>11</v>
+      </c>
+      <c r="E986">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="987" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A987" t="s">
+        <v>5</v>
+      </c>
+      <c r="B987" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C987" t="s">
+        <v>37</v>
+      </c>
+      <c r="D987" t="s">
+        <v>11</v>
+      </c>
+      <c r="E987">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="988" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A988" t="s">
+        <v>5</v>
+      </c>
+      <c r="B988" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C988" t="s">
+        <v>37</v>
+      </c>
+      <c r="D988" t="s">
+        <v>11</v>
+      </c>
+      <c r="E988">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
we added so mo data
</commit_message>
<xml_diff>
--- a/raw_data/pv_curves.xlsx
+++ b/raw_data/pv_curves.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3497" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3780" uniqueCount="40">
   <si>
     <t>species</t>
   </si>
@@ -138,6 +138,12 @@
   </si>
   <si>
     <t>thelypteris_nicaraguensis</t>
+  </si>
+  <si>
+    <t>elaphoglossum_latifolia</t>
+  </si>
+  <si>
+    <t>18/7/2017</t>
   </si>
 </sst>
 </file>
@@ -500,18 +506,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P988"/>
+  <dimension ref="A1:P1057"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A948" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E967" sqref="E967"/>
+      <pane ySplit="1" topLeftCell="A967" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I981" sqref="I981"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="9.140625" style="1"/>
     <col min="6" max="6" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
@@ -24681,9 +24687,14 @@
         <v>11</v>
       </c>
       <c r="E966">
-        <v>8</v>
-      </c>
-      <c r="G966" s="3"/>
+        <v>4</v>
+      </c>
+      <c r="F966" s="3">
+        <v>0.91649999999999998</v>
+      </c>
+      <c r="G966" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="967" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A967" t="s">
@@ -24699,7 +24710,13 @@
         <v>11</v>
       </c>
       <c r="E967">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F967" s="3">
+        <v>0.89529999999999998</v>
+      </c>
+      <c r="G967" s="3">
+        <v>2.8</v>
       </c>
     </row>
     <row r="968" spans="1:7" x14ac:dyDescent="0.25">
@@ -24716,7 +24733,13 @@
         <v>11</v>
       </c>
       <c r="E968">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F968" s="3">
+        <v>0.88360000000000005</v>
+      </c>
+      <c r="G968" s="3">
+        <v>6</v>
       </c>
     </row>
     <row r="969" spans="1:7" x14ac:dyDescent="0.25">
@@ -24733,7 +24756,13 @@
         <v>11</v>
       </c>
       <c r="E969">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F969" s="3">
+        <v>0.87549999999999994</v>
+      </c>
+      <c r="G969" s="3">
+        <v>10</v>
       </c>
     </row>
     <row r="970" spans="1:7" x14ac:dyDescent="0.25">
@@ -24750,7 +24779,13 @@
         <v>11</v>
       </c>
       <c r="E970">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F970" s="3">
+        <v>0.86509999999999998</v>
+      </c>
+      <c r="G970" s="3">
+        <v>13</v>
       </c>
     </row>
     <row r="971" spans="1:7" x14ac:dyDescent="0.25">
@@ -24767,7 +24802,13 @@
         <v>11</v>
       </c>
       <c r="E971">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F971" s="3">
+        <v>0.84609999999999996</v>
+      </c>
+      <c r="G971" s="3">
+        <v>13.9</v>
       </c>
     </row>
     <row r="972" spans="1:7" x14ac:dyDescent="0.25">
@@ -24784,7 +24825,13 @@
         <v>11</v>
       </c>
       <c r="E972">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F972" s="3">
+        <v>0.82769999999999999</v>
+      </c>
+      <c r="G972" s="3">
+        <v>15</v>
       </c>
     </row>
     <row r="973" spans="1:7" x14ac:dyDescent="0.25">
@@ -24801,7 +24848,13 @@
         <v>11</v>
       </c>
       <c r="E973">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F973" s="3">
+        <v>0.79810000000000003</v>
+      </c>
+      <c r="G973" s="3">
+        <v>15</v>
       </c>
     </row>
     <row r="974" spans="1:7" x14ac:dyDescent="0.25">
@@ -24818,7 +24871,13 @@
         <v>11</v>
       </c>
       <c r="E974">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F974" s="3">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="G974" s="3">
+        <v>17</v>
       </c>
     </row>
     <row r="975" spans="1:7" x14ac:dyDescent="0.25">
@@ -24835,7 +24894,13 @@
         <v>11</v>
       </c>
       <c r="E975">
-        <v>8</v>
+        <v>4</v>
+      </c>
+      <c r="F975" s="3">
+        <v>0.69220000000000004</v>
+      </c>
+      <c r="G975" s="3">
+        <v>18.5</v>
       </c>
     </row>
     <row r="976" spans="1:7" x14ac:dyDescent="0.25">
@@ -24843,220 +24908,1885 @@
         <v>5</v>
       </c>
       <c r="B976" s="4" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C976" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D976" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E976">
+        <v>1</v>
+      </c>
+      <c r="F976" s="3">
+        <v>0.93020000000000003</v>
+      </c>
+      <c r="G976" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="977" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A977" t="s">
+        <v>5</v>
+      </c>
+      <c r="B977" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C977" t="s">
+        <v>38</v>
+      </c>
+      <c r="D977" t="s">
+        <v>6</v>
+      </c>
+      <c r="E977">
+        <v>1</v>
+      </c>
+      <c r="F977" s="3">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="G977" s="3">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="978" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A978" t="s">
+        <v>5</v>
+      </c>
+      <c r="B978" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C978" t="s">
+        <v>38</v>
+      </c>
+      <c r="D978" t="s">
+        <v>6</v>
+      </c>
+      <c r="E978">
+        <v>1</v>
+      </c>
+      <c r="F978" s="3">
+        <v>0.92510000000000003</v>
+      </c>
+      <c r="G978" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="979" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A979" t="s">
+        <v>5</v>
+      </c>
+      <c r="B979" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C979" t="s">
+        <v>38</v>
+      </c>
+      <c r="D979" t="s">
+        <v>6</v>
+      </c>
+      <c r="E979">
+        <v>1</v>
+      </c>
+      <c r="F979" s="3">
+        <v>0.92330000000000001</v>
+      </c>
+      <c r="G979" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="980" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A980" t="s">
+        <v>5</v>
+      </c>
+      <c r="B980" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C980" t="s">
+        <v>38</v>
+      </c>
+      <c r="D980" t="s">
+        <v>6</v>
+      </c>
+      <c r="E980">
+        <v>1</v>
+      </c>
+      <c r="F980" s="3">
+        <v>0.9214</v>
+      </c>
+      <c r="G980" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="981" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A981" t="s">
+        <v>5</v>
+      </c>
+      <c r="B981" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C981" t="s">
+        <v>38</v>
+      </c>
+      <c r="D981" t="s">
+        <v>6</v>
+      </c>
+      <c r="E981">
+        <v>1</v>
+      </c>
+      <c r="F981" s="3">
+        <v>0.92</v>
+      </c>
+      <c r="G981" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="982" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A982" t="s">
+        <v>5</v>
+      </c>
+      <c r="B982" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C982" t="s">
+        <v>38</v>
+      </c>
+      <c r="D982" t="s">
+        <v>6</v>
+      </c>
+      <c r="E982">
+        <v>1</v>
+      </c>
+      <c r="F982" s="3">
+        <v>0.9194</v>
+      </c>
+      <c r="G982" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="983" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A983" t="s">
+        <v>5</v>
+      </c>
+      <c r="B983" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C983" t="s">
+        <v>38</v>
+      </c>
+      <c r="D983" t="s">
+        <v>6</v>
+      </c>
+      <c r="E983">
+        <v>1</v>
+      </c>
+      <c r="F983" s="3">
+        <v>0.91779999999999995</v>
+      </c>
+      <c r="G983" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="984" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A984" t="s">
+        <v>5</v>
+      </c>
+      <c r="B984" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C984" t="s">
+        <v>38</v>
+      </c>
+      <c r="D984" t="s">
+        <v>6</v>
+      </c>
+      <c r="E984">
+        <v>1</v>
+      </c>
+      <c r="F984" s="3">
+        <v>0.91239999999999999</v>
+      </c>
+      <c r="G984" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="985" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A985" t="s">
+        <v>5</v>
+      </c>
+      <c r="B985" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C985" t="s">
+        <v>38</v>
+      </c>
+      <c r="D985" t="s">
+        <v>6</v>
+      </c>
+      <c r="E985">
+        <v>1</v>
+      </c>
+      <c r="F985" s="3">
+        <v>0.90549999999999997</v>
+      </c>
+      <c r="G985" s="3">
+        <v>13.2</v>
+      </c>
+    </row>
+    <row r="986" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A986" t="s">
+        <v>5</v>
+      </c>
+      <c r="B986" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C986" t="s">
+        <v>38</v>
+      </c>
+      <c r="D986" t="s">
+        <v>6</v>
+      </c>
+      <c r="E986">
+        <v>1</v>
+      </c>
+      <c r="F986" s="3">
+        <v>0.89690000000000003</v>
+      </c>
+      <c r="G986" s="3">
+        <v>14.4</v>
+      </c>
+    </row>
+    <row r="987" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A987" t="s">
+        <v>5</v>
+      </c>
+      <c r="B987" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C987" t="s">
+        <v>38</v>
+      </c>
+      <c r="D987" t="s">
+        <v>6</v>
+      </c>
+      <c r="E987">
+        <v>1</v>
+      </c>
+      <c r="F987" s="3">
+        <v>0.88970000000000005</v>
+      </c>
+      <c r="G987" s="3">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="988" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A988" t="s">
+        <v>5</v>
+      </c>
+      <c r="B988" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C988" t="s">
+        <v>38</v>
+      </c>
+      <c r="D988" t="s">
+        <v>6</v>
+      </c>
+      <c r="E988">
+        <v>2</v>
+      </c>
+      <c r="F988" s="3">
+        <v>1.3132999999999999</v>
+      </c>
+      <c r="G988" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="989" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A989" t="s">
+        <v>5</v>
+      </c>
+      <c r="B989" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C989" t="s">
+        <v>38</v>
+      </c>
+      <c r="D989" t="s">
+        <v>6</v>
+      </c>
+      <c r="E989">
+        <v>2</v>
+      </c>
+      <c r="F989" s="3">
+        <v>1.3083</v>
+      </c>
+      <c r="G989" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="990" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A990" t="s">
+        <v>5</v>
+      </c>
+      <c r="B990" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C990" t="s">
+        <v>38</v>
+      </c>
+      <c r="D990" t="s">
+        <v>6</v>
+      </c>
+      <c r="E990">
+        <v>2</v>
+      </c>
+      <c r="F990" s="3">
+        <v>1.3052999999999999</v>
+      </c>
+      <c r="G990" s="3">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="991" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A991" t="s">
+        <v>5</v>
+      </c>
+      <c r="B991" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C991" t="s">
+        <v>38</v>
+      </c>
+      <c r="D991" t="s">
+        <v>6</v>
+      </c>
+      <c r="E991">
+        <v>2</v>
+      </c>
+      <c r="F991" s="3">
+        <v>1.3009999999999999</v>
+      </c>
+      <c r="G991" s="3">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="992" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A992" t="s">
+        <v>5</v>
+      </c>
+      <c r="B992" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C992" t="s">
+        <v>38</v>
+      </c>
+      <c r="D992" t="s">
+        <v>6</v>
+      </c>
+      <c r="E992">
+        <v>2</v>
+      </c>
+      <c r="F992" s="3">
+        <v>1.2981</v>
+      </c>
+      <c r="G992" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="993" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A993" t="s">
+        <v>5</v>
+      </c>
+      <c r="B993" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C993" t="s">
+        <v>38</v>
+      </c>
+      <c r="D993" t="s">
+        <v>6</v>
+      </c>
+      <c r="E993">
+        <v>2</v>
+      </c>
+      <c r="F993" s="3">
+        <v>1.2949999999999999</v>
+      </c>
+      <c r="G993" s="3">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="994" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A994" t="s">
+        <v>5</v>
+      </c>
+      <c r="B994" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C994" t="s">
+        <v>38</v>
+      </c>
+      <c r="D994" t="s">
+        <v>6</v>
+      </c>
+      <c r="E994">
+        <v>2</v>
+      </c>
+      <c r="F994" s="3">
+        <v>1.2922</v>
+      </c>
+      <c r="G994" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="995" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A995" t="s">
+        <v>5</v>
+      </c>
+      <c r="B995" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C995" t="s">
+        <v>38</v>
+      </c>
+      <c r="D995" t="s">
+        <v>6</v>
+      </c>
+      <c r="E995">
+        <v>2</v>
+      </c>
+      <c r="F995" s="3">
+        <v>1.2895000000000001</v>
+      </c>
+      <c r="G995" s="3">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="996" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A996" t="s">
+        <v>5</v>
+      </c>
+      <c r="B996" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C996" t="s">
+        <v>38</v>
+      </c>
+      <c r="D996" t="s">
+        <v>6</v>
+      </c>
+      <c r="E996">
+        <v>2</v>
+      </c>
+      <c r="F996" s="3">
+        <v>1.2862</v>
+      </c>
+      <c r="G996" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="997" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A997" t="s">
+        <v>5</v>
+      </c>
+      <c r="B997" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C997" t="s">
+        <v>38</v>
+      </c>
+      <c r="D997" t="s">
+        <v>6</v>
+      </c>
+      <c r="E997">
+        <v>2</v>
+      </c>
+      <c r="F997" s="3">
+        <v>1.2836000000000001</v>
+      </c>
+      <c r="G997" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="998" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A998" t="s">
+        <v>5</v>
+      </c>
+      <c r="B998" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C998" t="s">
+        <v>38</v>
+      </c>
+      <c r="D998" t="s">
+        <v>6</v>
+      </c>
+      <c r="E998">
+        <v>2</v>
+      </c>
+      <c r="F998" s="3">
+        <v>1.2810999999999999</v>
+      </c>
+      <c r="G998" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="999" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A999" t="s">
+        <v>5</v>
+      </c>
+      <c r="B999" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C999" t="s">
+        <v>38</v>
+      </c>
+      <c r="D999" t="s">
+        <v>6</v>
+      </c>
+      <c r="E999">
+        <v>2</v>
+      </c>
+      <c r="F999" s="3">
+        <v>1.2705</v>
+      </c>
+      <c r="G999" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1000" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1000" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1000" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1000" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1000" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1000">
+        <v>2</v>
+      </c>
+      <c r="F1000" s="3">
+        <v>1.2649999999999999</v>
+      </c>
+      <c r="G1000" s="3">
+        <v>10.199999999999999</v>
+      </c>
+    </row>
+    <row r="1001" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1001" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1001" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1001" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1001" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1001">
+        <v>2</v>
+      </c>
+      <c r="F1001" s="3">
+        <v>1.2326999999999999</v>
+      </c>
+      <c r="G1001" s="3">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="1002" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1002" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1002" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1002" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1002" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1002">
+        <v>2</v>
+      </c>
+      <c r="F1002" s="3">
+        <v>1.2209000000000001</v>
+      </c>
+      <c r="G1002" s="3">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="1003" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1003" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1003" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1003" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1003" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1003">
+        <v>2</v>
+      </c>
+      <c r="F1003" s="3">
+        <v>1.2108000000000001</v>
+      </c>
+      <c r="G1003" s="3">
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="1004" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1004" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1004" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1004" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1004" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1004">
+        <v>3</v>
+      </c>
+      <c r="F1004" s="3">
+        <v>1.8383</v>
+      </c>
+      <c r="G1004" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1005" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1005" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1005" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1005" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1005" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1005">
+        <v>3</v>
+      </c>
+      <c r="F1005" s="3">
+        <v>1.8262</v>
+      </c>
+      <c r="G1005" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1006" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1006" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1006" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1006" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1006" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1006">
+        <v>3</v>
+      </c>
+      <c r="F1006" s="3">
+        <v>1.8199000000000001</v>
+      </c>
+      <c r="G1006" s="3">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="1007" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1007" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1007" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1007" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1007" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1007">
+        <v>3</v>
+      </c>
+      <c r="F1007" s="3">
+        <v>1.8166</v>
+      </c>
+      <c r="G1007" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1008" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1008" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1008" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1008" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1008" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1008">
+        <v>3</v>
+      </c>
+      <c r="F1008" s="3">
+        <v>1.8142</v>
+      </c>
+      <c r="G1008" s="3">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="1009" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1009" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1009" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1009" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1009" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1009">
+        <v>3</v>
+      </c>
+      <c r="F1009" s="3">
+        <v>1.8136000000000001</v>
+      </c>
+      <c r="G1009" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1010" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1010" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1010" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1010" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1010" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1010">
+        <v>3</v>
+      </c>
+      <c r="F1010" s="3">
+        <v>1.8078000000000001</v>
+      </c>
+      <c r="G1010" s="3">
+        <v>9.8000000000000007</v>
+      </c>
+    </row>
+    <row r="1011" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1011" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1011" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1011" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1011" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1011">
+        <v>3</v>
+      </c>
+      <c r="F1011" s="3">
+        <v>1.8053999999999999</v>
+      </c>
+      <c r="G1011" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1012" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1012" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1012" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1012" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1012" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1012">
+        <v>3</v>
+      </c>
+      <c r="F1012" s="3">
+        <v>1.8026</v>
+      </c>
+      <c r="G1012" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1013" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1013" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1013" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1013" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1013" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1013">
+        <v>3</v>
+      </c>
+      <c r="F1013" s="3">
+        <v>1.7979000000000001</v>
+      </c>
+      <c r="G1013" s="3">
+        <v>13.4</v>
+      </c>
+    </row>
+    <row r="1014" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1014" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1014" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1014" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1014" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1014">
+        <v>3</v>
+      </c>
+      <c r="F1014" s="3">
+        <v>1.788</v>
+      </c>
+      <c r="G1014" s="3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1015" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1015" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1015" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1015" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1015" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1015">
+        <v>4</v>
+      </c>
+      <c r="F1015" s="3">
+        <v>1.7586999999999999</v>
+      </c>
+      <c r="G1015" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1016" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1016" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1016" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1016" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1016" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1016">
+        <v>4</v>
+      </c>
+      <c r="F1016" s="3">
+        <v>1.7538</v>
+      </c>
+      <c r="G1016" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="1017" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1017" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1017" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1017" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1017" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1017">
+        <v>4</v>
+      </c>
+      <c r="F1017" s="3">
+        <v>1.7464</v>
+      </c>
+      <c r="G1017" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1018" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1018" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1018" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1018" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1018" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1018">
+        <v>4</v>
+      </c>
+      <c r="F1018" s="3">
+        <v>1.7438</v>
+      </c>
+      <c r="G1018" s="3">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="1019" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1019" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1019" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1019" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1019" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1019">
+        <v>4</v>
+      </c>
+      <c r="F1019" s="3">
+        <v>1.7398</v>
+      </c>
+      <c r="G1019" s="3">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="1020" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1020" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1020" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1020" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1020" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1020">
+        <v>4</v>
+      </c>
+      <c r="F1020" s="3">
+        <v>1.7375</v>
+      </c>
+      <c r="G1020" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1021" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1021" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1021" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1021" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1021" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1021">
+        <v>4</v>
+      </c>
+      <c r="F1021" s="3">
+        <v>1.7342</v>
+      </c>
+      <c r="G1021" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1022" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1022" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1022" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1022" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1022" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1022">
+        <v>4</v>
+      </c>
+      <c r="F1022" s="3">
+        <v>1.7312000000000001</v>
+      </c>
+      <c r="G1022" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1023" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1023" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1023" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1023" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1023" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1023">
+        <v>4</v>
+      </c>
+      <c r="F1023" s="3">
+        <v>1.7283999999999999</v>
+      </c>
+      <c r="G1023" s="3">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="1024" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1024" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1024" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1024" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1024" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1024">
+        <v>4</v>
+      </c>
+      <c r="F1024" s="3">
+        <v>1.7237</v>
+      </c>
+      <c r="G1024" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="977" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A977" t="s">
-        <v>5</v>
-      </c>
-      <c r="B977" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C977" t="s">
-        <v>37</v>
-      </c>
-      <c r="D977" t="s">
-        <v>11</v>
-      </c>
-      <c r="E977">
+    <row r="1025" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1025" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1025" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1025" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1025" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1025">
+        <v>4</v>
+      </c>
+      <c r="F1025" s="3">
+        <v>1.7191000000000001</v>
+      </c>
+      <c r="G1025" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1026" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1026" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1026" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1026" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1026">
+        <v>4</v>
+      </c>
+      <c r="F1026" s="3">
+        <v>1.7084999999999999</v>
+      </c>
+      <c r="G1026" s="3">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1027" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1027" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1027" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1027" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1027">
+        <v>4</v>
+      </c>
+      <c r="F1027" s="3">
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="G1027" s="3">
+        <v>11.1</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1028" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1028" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1028" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1028" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1028">
+        <v>4</v>
+      </c>
+      <c r="F1028" s="3">
+        <v>1.6890000000000001</v>
+      </c>
+      <c r="G1028" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1029" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1029" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1029" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1029" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1029">
+        <v>4</v>
+      </c>
+      <c r="F1029" s="3">
+        <v>1.6819999999999999</v>
+      </c>
+      <c r="G1029" s="3">
+        <v>12.8</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1030" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1030" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1030" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1030" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1030">
+        <v>4</v>
+      </c>
+      <c r="F1030" s="3">
+        <v>1.6636</v>
+      </c>
+      <c r="G1030" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1031" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1031" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1031" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1031" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1031">
+        <v>5</v>
+      </c>
+      <c r="F1031" s="3">
+        <v>2.3096000000000001</v>
+      </c>
+      <c r="G1031" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1032" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1032" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1032" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1032" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1032">
+        <v>5</v>
+      </c>
+      <c r="F1032" s="3">
+        <v>2.2900999999999998</v>
+      </c>
+      <c r="G1032" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1033" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1033" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1033" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1033" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1033">
+        <v>5</v>
+      </c>
+      <c r="F1033" s="3">
+        <v>2.2856000000000001</v>
+      </c>
+      <c r="G1033" s="3">
+        <v>2.6</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1034" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1034" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1034" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1034" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1034">
+        <v>5</v>
+      </c>
+      <c r="F1034" s="3">
+        <v>2.2827000000000002</v>
+      </c>
+      <c r="G1034" s="3">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="1035" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1035" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1035" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1035" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1035" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1035">
+        <v>5</v>
+      </c>
+      <c r="F1035" s="3">
+        <v>2.2808000000000002</v>
+      </c>
+      <c r="G1035" s="3">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="1036" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1036" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1036" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1036" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1036" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1036">
+        <v>5</v>
+      </c>
+      <c r="F1036" s="3">
+        <v>2.2787000000000002</v>
+      </c>
+      <c r="G1036" s="3">
+        <v>4.7</v>
+      </c>
+    </row>
+    <row r="1037" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1037" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1037" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1037" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1037" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1037">
+        <v>5</v>
+      </c>
+      <c r="F1037" s="3">
+        <v>2.2764000000000002</v>
+      </c>
+      <c r="G1037" s="3">
+        <v>4.8</v>
+      </c>
+    </row>
+    <row r="1038" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1038" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1038" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1038" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1038" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1038">
+        <v>5</v>
+      </c>
+      <c r="F1038" s="3">
+        <v>2.2751999999999999</v>
+      </c>
+      <c r="G1038" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1039" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1039" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1039" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1039" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1039" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1039">
+        <v>5</v>
+      </c>
+      <c r="F1039" s="3">
+        <v>2.2746</v>
+      </c>
+      <c r="G1039" s="3">
+        <v>5.9</v>
+      </c>
+    </row>
+    <row r="1040" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1040" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1040" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1040" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1040" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1040">
+        <v>5</v>
+      </c>
+      <c r="F1040" s="3">
+        <v>2.2692999999999999</v>
+      </c>
+      <c r="G1040" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="978" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A978" t="s">
-        <v>5</v>
-      </c>
-      <c r="B978" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C978" t="s">
-        <v>37</v>
-      </c>
-      <c r="D978" t="s">
-        <v>11</v>
-      </c>
-      <c r="E978">
+    <row r="1041" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1041" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1041" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1041" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1041" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1041">
+        <v>5</v>
+      </c>
+      <c r="F1041" s="3">
+        <v>2.2667000000000002</v>
+      </c>
+      <c r="G1041" s="3">
         <v>8</v>
       </c>
     </row>
-    <row r="979" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A979" t="s">
-        <v>5</v>
-      </c>
-      <c r="B979" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C979" t="s">
-        <v>37</v>
-      </c>
-      <c r="D979" t="s">
-        <v>11</v>
-      </c>
-      <c r="E979">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="980" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A980" t="s">
-        <v>5</v>
-      </c>
-      <c r="B980" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C980" t="s">
-        <v>37</v>
-      </c>
-      <c r="D980" t="s">
-        <v>11</v>
-      </c>
-      <c r="E980">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="981" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A981" t="s">
-        <v>5</v>
-      </c>
-      <c r="B981" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C981" t="s">
-        <v>37</v>
-      </c>
-      <c r="D981" t="s">
-        <v>11</v>
-      </c>
-      <c r="E981">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="982" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A982" t="s">
-        <v>5</v>
-      </c>
-      <c r="B982" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C982" t="s">
-        <v>37</v>
-      </c>
-      <c r="D982" t="s">
-        <v>11</v>
-      </c>
-      <c r="E982">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="983" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A983" t="s">
-        <v>5</v>
-      </c>
-      <c r="B983" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C983" t="s">
-        <v>37</v>
-      </c>
-      <c r="D983" t="s">
-        <v>11</v>
-      </c>
-      <c r="E983">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="984" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A984" t="s">
-        <v>5</v>
-      </c>
-      <c r="B984" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C984" t="s">
-        <v>37</v>
-      </c>
-      <c r="D984" t="s">
-        <v>11</v>
-      </c>
-      <c r="E984">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="985" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A985" t="s">
-        <v>5</v>
-      </c>
-      <c r="B985" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C985" t="s">
-        <v>37</v>
-      </c>
-      <c r="D985" t="s">
-        <v>11</v>
-      </c>
-      <c r="E985">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="986" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A986" t="s">
-        <v>5</v>
-      </c>
-      <c r="B986" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C986" t="s">
-        <v>37</v>
-      </c>
-      <c r="D986" t="s">
-        <v>11</v>
-      </c>
-      <c r="E986">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="987" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A987" t="s">
-        <v>5</v>
-      </c>
-      <c r="B987" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C987" t="s">
-        <v>37</v>
-      </c>
-      <c r="D987" t="s">
-        <v>11</v>
-      </c>
-      <c r="E987">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="988" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A988" t="s">
-        <v>5</v>
-      </c>
-      <c r="B988" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="C988" t="s">
-        <v>37</v>
-      </c>
-      <c r="D988" t="s">
-        <v>11</v>
-      </c>
-      <c r="E988">
-        <v>8</v>
+    <row r="1042" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1042" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1042" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1042" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1042" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1042">
+        <v>5</v>
+      </c>
+      <c r="F1042" s="3">
+        <v>2.2589999999999999</v>
+      </c>
+      <c r="G1042" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1043" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1043" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1043" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1043" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1043" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1043">
+        <v>5</v>
+      </c>
+      <c r="F1043" s="3">
+        <v>2.2469999999999999</v>
+      </c>
+      <c r="G1043" s="3">
+        <v>14.9</v>
+      </c>
+    </row>
+    <row r="1044" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1044" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1044" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1044" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1044" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1044">
+        <v>5</v>
+      </c>
+      <c r="F1044" s="3">
+        <v>2.2357</v>
+      </c>
+      <c r="G1044" s="3">
+        <v>15.1</v>
+      </c>
+    </row>
+    <row r="1045" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1045" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1045" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1045" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1045" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1045">
+        <v>5</v>
+      </c>
+      <c r="F1045" s="3">
+        <v>2.2610000000000001</v>
+      </c>
+      <c r="G1045" s="3">
+        <v>17.899999999999999</v>
+      </c>
+    </row>
+    <row r="1046" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1046" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1046" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1046" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1046" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1046">
+        <v>6</v>
+      </c>
+      <c r="F1046" s="3">
+        <v>1.8929</v>
+      </c>
+      <c r="G1046" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="1047" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1047" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1047" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1047" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1047" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1047">
+        <v>6</v>
+      </c>
+      <c r="F1047" s="3">
+        <v>1.8852</v>
+      </c>
+      <c r="G1047" s="3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="1048" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1048" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1048" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1048" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1048" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1048">
+        <v>6</v>
+      </c>
+      <c r="F1048" s="3">
+        <v>1.8764000000000001</v>
+      </c>
+      <c r="G1048" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1049" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1049" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1049" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1049" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1049" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1049">
+        <v>6</v>
+      </c>
+      <c r="F1049" s="3">
+        <v>1.8697999999999999</v>
+      </c>
+      <c r="G1049" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1050" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1050" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1050" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1050" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1050" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1050">
+        <v>6</v>
+      </c>
+      <c r="F1050" s="3">
+        <v>1.8615999999999999</v>
+      </c>
+      <c r="G1050" s="3">
+        <v>6.2</v>
+      </c>
+    </row>
+    <row r="1051" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1051" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1051" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1051" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1051" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1051">
+        <v>6</v>
+      </c>
+      <c r="F1051" s="3">
+        <v>1.8565</v>
+      </c>
+      <c r="G1051" s="3">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="1052" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1052" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1052" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1052" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1052" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1052">
+        <v>6</v>
+      </c>
+      <c r="F1052" s="3">
+        <v>1.8501000000000001</v>
+      </c>
+      <c r="G1052" s="3">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="1053" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1053" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1053" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1053" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1053" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1053">
+        <v>6</v>
+      </c>
+      <c r="F1053" s="3">
+        <v>1.8376999999999999</v>
+      </c>
+      <c r="G1053" s="3">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1054" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1054" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1054" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1054" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1054">
+        <v>6</v>
+      </c>
+      <c r="F1054" s="3">
+        <v>1.8238000000000001</v>
+      </c>
+      <c r="G1054" s="3">
+        <v>10.3</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1055" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1055" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1055" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1055" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1055">
+        <v>6</v>
+      </c>
+      <c r="F1055" s="3">
+        <v>1.8089999999999999</v>
+      </c>
+      <c r="G1055" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1056" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1056" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1056" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1056" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1056">
+        <v>6</v>
+      </c>
+      <c r="F1056" s="3">
+        <v>1.7875000000000001</v>
+      </c>
+      <c r="G1056" s="3">
+        <v>13.5</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1057" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1057" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1057" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1057" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1057">
+        <v>6</v>
+      </c>
+      <c r="F1057" s="3">
+        <v>1.766</v>
+      </c>
+      <c r="G1057" s="3">
+        <v>13.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>